<commit_message>
Reading LCA from Excel
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1896157\OneDrive - University of Edinburgh\Rafael\Models\MaxProfitFeeding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1896157_ed_ac_uk/Documents/Rafael/Models/GreenFeeding/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,8 +14,10 @@
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
     <sheet name="Scenario" sheetId="3" r:id="rId2"/>
-    <sheet name="FeedLibrary" sheetId="1" r:id="rId3"/>
-    <sheet name="Parameters List" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="LCA" sheetId="5" r:id="rId3"/>
+    <sheet name="LCA Library" sheetId="6" r:id="rId4"/>
+    <sheet name="Feed Library" sheetId="1" r:id="rId5"/>
+    <sheet name="Parameters List" sheetId="4" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="345">
   <si>
     <t>IFN</t>
   </si>
@@ -1031,10 +1033,37 @@
     <t>Linearization factor</t>
   </si>
   <si>
-    <t>LCA</t>
+    <t>Cost</t>
   </si>
   <si>
-    <t>Cost</t>
+    <t>E-BF</t>
+  </si>
+  <si>
+    <t>LCA_GHG_weight</t>
+  </si>
+  <si>
+    <t>LCA_GHG</t>
+  </si>
+  <si>
+    <t>LCA_cost</t>
+  </si>
+  <si>
+    <t>Epislon</t>
+  </si>
+  <si>
+    <t>LCA_weight</t>
+  </si>
+  <si>
+    <t>Methane</t>
+  </si>
+  <si>
+    <t>IPCC2006</t>
+  </si>
+  <si>
+    <t>Methane_Equation</t>
+  </si>
+  <si>
+    <t>LCA_ID</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1">
@@ -1226,14 +1255,62 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="74">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1546,6 +1623,39 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -1584,56 +1694,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1648,17 +1708,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:E13" totalsRowShown="0" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:E13" totalsRowShown="0" dataDxfId="5">
   <autoFilter ref="A1:E13"/>
   <sortState ref="A2:E30">
     <sortCondition ref="A1:A30"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="68"/>
-    <tableColumn id="2" name="Min" dataDxfId="67"/>
-    <tableColumn id="3" name="Max" dataDxfId="66"/>
-    <tableColumn id="4" name="Cost" dataDxfId="65"/>
-    <tableColumn id="5" name="Name" dataDxfId="64">
+    <tableColumn id="1" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" name="Min" dataDxfId="3"/>
+    <tableColumn id="3" name="Max" dataDxfId="2"/>
+    <tableColumn id="4" name="Cost" dataDxfId="1"/>
+    <tableColumn id="5" name="Name" dataDxfId="0">
       <calculatedColumnFormula>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1667,7 +1727,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="63" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="73" tableBorderDxfId="72">
   <autoFilter ref="A1:Q3"/>
   <tableColumns count="17">
     <tableColumn id="1" name="ID"/>
@@ -1686,77 +1746,111 @@
     <tableColumn id="14" name="LB"/>
     <tableColumn id="15" name="UB"/>
     <tableColumn id="16" name="Tol"/>
-    <tableColumn id="17" name="LCA"/>
+    <tableColumn id="17" name="LCA_ID"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:BF219" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:H2" totalsRowShown="0">
+  <autoFilter ref="A1:H2"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="LCA_cost"/>
+    <tableColumn id="3" name="Epislon"/>
+    <tableColumn id="4" name="LCA_weight"/>
+    <tableColumn id="5" name="LCA_GHG"/>
+    <tableColumn id="6" name="LCA_GHG_weight"/>
+    <tableColumn id="7" name="Methane"/>
+    <tableColumn id="8" name="Methane_Equation"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela26" displayName="Tabela26" ref="A1:C13" totalsRowShown="0" dataDxfId="71">
+  <autoFilter ref="A1:C13"/>
+  <sortState ref="A2:E30">
+    <sortCondition ref="A1:A30"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" name="ID" dataDxfId="70"/>
+    <tableColumn id="5" name="Name" dataDxfId="69">
+      <calculatedColumnFormula>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="LCA_GHG" dataDxfId="68"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:BF219" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <autoFilter ref="A1:BF219"/>
   <sortState ref="A2:BF219">
     <sortCondition ref="A4:A5"/>
   </sortState>
   <tableColumns count="58">
-    <tableColumn id="1" name="ID" dataDxfId="57"/>
-    <tableColumn id="2" name="Feed" dataDxfId="56"/>
-    <tableColumn id="4" name="IFN" dataDxfId="55"/>
-    <tableColumn id="5" name="Cost, $/Tonne AF" dataDxfId="54"/>
-    <tableColumn id="7" name="Forage, %DM" dataDxfId="53"/>
-    <tableColumn id="8" name="DM, %AF" dataDxfId="52"/>
-    <tableColumn id="16" name="CP, %DM" dataDxfId="51"/>
-    <tableColumn id="31" name="SP, %CP" dataDxfId="50"/>
-    <tableColumn id="29" name="ADICP, %CP" dataDxfId="49"/>
-    <tableColumn id="24" name="Sugars, %DM" dataDxfId="48"/>
-    <tableColumn id="25" name="OA, %DM" dataDxfId="47"/>
-    <tableColumn id="23" name="Fat, %DM" dataDxfId="46"/>
-    <tableColumn id="9" name="Ash, %DM" dataDxfId="45"/>
-    <tableColumn id="10" name="Starch, %DM" dataDxfId="44"/>
-    <tableColumn id="12" name="NDF, %DM" dataDxfId="43"/>
-    <tableColumn id="13" name="Lignin, %DM" dataDxfId="42"/>
-    <tableColumn id="14" name="TDN, %DM" dataDxfId="41"/>
-    <tableColumn id="15" name="ME, Mcal/kg" dataDxfId="40"/>
-    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="39"/>
-    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="38"/>
-    <tableColumn id="21" name="RUP, %CP" dataDxfId="37"/>
-    <tableColumn id="22" name="kd PB, %/h" dataDxfId="36"/>
-    <tableColumn id="26" name="kd CB1, %/h" dataDxfId="35"/>
-    <tableColumn id="27" name="kd CB2, %/h" dataDxfId="34"/>
-    <tableColumn id="17" name="kd CB3, %/h" dataDxfId="33"/>
-    <tableColumn id="28" name="PBID, %" dataDxfId="32"/>
-    <tableColumn id="6" name="CB1ID, %" dataDxfId="31"/>
-    <tableColumn id="3" name="CB2ID, %" dataDxfId="30"/>
-    <tableColumn id="20" name="pef, %NDF" dataDxfId="29"/>
-    <tableColumn id="11" name="ARG, %DM" dataDxfId="28"/>
-    <tableColumn id="32" name="HIS, %DM" dataDxfId="27"/>
-    <tableColumn id="33" name="ILE, %DM" dataDxfId="26"/>
-    <tableColumn id="34" name="LEU, %DM" dataDxfId="25"/>
-    <tableColumn id="35" name="LYS, %DM" dataDxfId="24"/>
-    <tableColumn id="36" name="MET, %DM" dataDxfId="23"/>
-    <tableColumn id="37" name="CYS, %DM" dataDxfId="22"/>
-    <tableColumn id="38" name="PHE, %DM" dataDxfId="21"/>
-    <tableColumn id="39" name="TYR, %DM" dataDxfId="20"/>
-    <tableColumn id="40" name="THR, %DM" dataDxfId="19"/>
-    <tableColumn id="41" name="TRP, %DM" dataDxfId="18"/>
-    <tableColumn id="42" name="VAL, %DM" dataDxfId="17"/>
-    <tableColumn id="43" name="Ca, % DM" dataDxfId="16"/>
-    <tableColumn id="44" name="P, % DM" dataDxfId="15"/>
-    <tableColumn id="45" name="Mg, % DM" dataDxfId="14"/>
-    <tableColumn id="46" name="Cl, % DM" dataDxfId="13"/>
-    <tableColumn id="47" name="K, % DM" dataDxfId="12"/>
-    <tableColumn id="48" name="Na, % DM" dataDxfId="11"/>
-    <tableColumn id="49" name="S, % DM" dataDxfId="10"/>
-    <tableColumn id="50" name="Co, mg/kg" dataDxfId="9"/>
-    <tableColumn id="51" name="Cu, mg/kg" dataDxfId="8"/>
-    <tableColumn id="52" name="I, mg/kg" dataDxfId="7"/>
-    <tableColumn id="53" name="Fe, mg/kg" dataDxfId="6"/>
-    <tableColumn id="54" name="Mn, mg/kg" dataDxfId="5"/>
-    <tableColumn id="55" name="Se, mg/kg" dataDxfId="4"/>
-    <tableColumn id="56" name="Zn, mg/kg" dataDxfId="3"/>
-    <tableColumn id="57" name="Vit A, IU/g" dataDxfId="2"/>
-    <tableColumn id="58" name="Vit D, IU/g" dataDxfId="1"/>
-    <tableColumn id="30" name="Vit E, IU/kg" dataDxfId="0"/>
+    <tableColumn id="1" name="ID" dataDxfId="63"/>
+    <tableColumn id="2" name="Feed" dataDxfId="62"/>
+    <tableColumn id="4" name="IFN" dataDxfId="61"/>
+    <tableColumn id="5" name="Cost, $/Tonne AF" dataDxfId="60"/>
+    <tableColumn id="7" name="Forage, %DM" dataDxfId="59"/>
+    <tableColumn id="8" name="DM, %AF" dataDxfId="58"/>
+    <tableColumn id="16" name="CP, %DM" dataDxfId="57"/>
+    <tableColumn id="31" name="SP, %CP" dataDxfId="56"/>
+    <tableColumn id="29" name="ADICP, %CP" dataDxfId="55"/>
+    <tableColumn id="24" name="Sugars, %DM" dataDxfId="54"/>
+    <tableColumn id="25" name="OA, %DM" dataDxfId="53"/>
+    <tableColumn id="23" name="Fat, %DM" dataDxfId="52"/>
+    <tableColumn id="9" name="Ash, %DM" dataDxfId="51"/>
+    <tableColumn id="10" name="Starch, %DM" dataDxfId="50"/>
+    <tableColumn id="12" name="NDF, %DM" dataDxfId="49"/>
+    <tableColumn id="13" name="Lignin, %DM" dataDxfId="48"/>
+    <tableColumn id="14" name="TDN, %DM" dataDxfId="47"/>
+    <tableColumn id="15" name="ME, Mcal/kg" dataDxfId="46"/>
+    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="45"/>
+    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="44"/>
+    <tableColumn id="21" name="RUP, %CP" dataDxfId="43"/>
+    <tableColumn id="22" name="kd PB, %/h" dataDxfId="42"/>
+    <tableColumn id="26" name="kd CB1, %/h" dataDxfId="41"/>
+    <tableColumn id="27" name="kd CB2, %/h" dataDxfId="40"/>
+    <tableColumn id="17" name="kd CB3, %/h" dataDxfId="39"/>
+    <tableColumn id="28" name="PBID, %" dataDxfId="38"/>
+    <tableColumn id="6" name="CB1ID, %" dataDxfId="37"/>
+    <tableColumn id="3" name="CB2ID, %" dataDxfId="36"/>
+    <tableColumn id="20" name="pef, %NDF" dataDxfId="35"/>
+    <tableColumn id="11" name="ARG, %DM" dataDxfId="34"/>
+    <tableColumn id="32" name="HIS, %DM" dataDxfId="33"/>
+    <tableColumn id="33" name="ILE, %DM" dataDxfId="32"/>
+    <tableColumn id="34" name="LEU, %DM" dataDxfId="31"/>
+    <tableColumn id="35" name="LYS, %DM" dataDxfId="30"/>
+    <tableColumn id="36" name="MET, %DM" dataDxfId="29"/>
+    <tableColumn id="37" name="CYS, %DM" dataDxfId="28"/>
+    <tableColumn id="38" name="PHE, %DM" dataDxfId="27"/>
+    <tableColumn id="39" name="TYR, %DM" dataDxfId="26"/>
+    <tableColumn id="40" name="THR, %DM" dataDxfId="25"/>
+    <tableColumn id="41" name="TRP, %DM" dataDxfId="24"/>
+    <tableColumn id="42" name="VAL, %DM" dataDxfId="23"/>
+    <tableColumn id="43" name="Ca, % DM" dataDxfId="22"/>
+    <tableColumn id="44" name="P, % DM" dataDxfId="21"/>
+    <tableColumn id="45" name="Mg, % DM" dataDxfId="20"/>
+    <tableColumn id="46" name="Cl, % DM" dataDxfId="19"/>
+    <tableColumn id="47" name="K, % DM" dataDxfId="18"/>
+    <tableColumn id="48" name="Na, % DM" dataDxfId="17"/>
+    <tableColumn id="49" name="S, % DM" dataDxfId="16"/>
+    <tableColumn id="50" name="Co, mg/kg" dataDxfId="15"/>
+    <tableColumn id="51" name="Cu, mg/kg" dataDxfId="14"/>
+    <tableColumn id="52" name="I, mg/kg" dataDxfId="13"/>
+    <tableColumn id="53" name="Fe, mg/kg" dataDxfId="12"/>
+    <tableColumn id="54" name="Mn, mg/kg" dataDxfId="11"/>
+    <tableColumn id="55" name="Se, mg/kg" dataDxfId="10"/>
+    <tableColumn id="56" name="Zn, mg/kg" dataDxfId="9"/>
+    <tableColumn id="57" name="Vit A, IU/g" dataDxfId="8"/>
+    <tableColumn id="58" name="Vit D, IU/g" dataDxfId="7"/>
+    <tableColumn id="30" name="Vit E, IU/kg" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2031,7 +2125,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2054,7 +2148,7 @@
         <v>314</v>
       </c>
       <c r="D1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E1" t="s">
         <v>325</v>
@@ -2292,7 +2386,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q13" sqref="O13:Q16"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2360,8 +2454,8 @@
       <c r="P1" s="28" t="s">
         <v>332</v>
       </c>
-      <c r="Q1" s="31" t="s">
-        <v>334</v>
+      <c r="Q1" s="29" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -2413,61 +2507,61 @@
       <c r="P2" s="23">
         <v>1E-3</v>
       </c>
-      <c r="Q2" t="b">
-        <v>0</v>
+      <c r="Q2">
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="29">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" t="s">
         <v>318</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3">
         <v>300</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3">
         <v>5</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" s="29">
-        <v>0</v>
-      </c>
-      <c r="I3" s="29">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>6.2</v>
       </c>
-      <c r="J3" s="29">
+      <c r="J3">
         <v>1.44</v>
       </c>
-      <c r="K3" s="30">
+      <c r="K3">
         <v>13.91</v>
       </c>
-      <c r="L3" s="29" t="s">
+      <c r="L3" t="s">
         <v>329</v>
       </c>
-      <c r="M3" s="29" t="s">
-        <v>329</v>
-      </c>
-      <c r="N3" s="29">
+      <c r="M3" t="s">
+        <v>335</v>
+      </c>
+      <c r="N3">
         <v>0.8</v>
       </c>
-      <c r="O3" s="29">
+      <c r="O3">
         <v>3</v>
       </c>
-      <c r="P3" s="29">
+      <c r="P3">
         <v>1E-3</v>
       </c>
-      <c r="Q3" t="b">
-        <v>0</v>
+      <c r="Q3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2481,11 +2575,242 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1" t="s">
+        <v>337</v>
+      </c>
+      <c r="F1" t="s">
+        <v>336</v>
+      </c>
+      <c r="G1" t="s">
+        <v>341</v>
+      </c>
+      <c r="H1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.05</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>34</v>
+      </c>
+      <c r="B2" s="17" t="str">
+        <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Citrus pulp, dry</v>
+      </c>
+      <c r="C2" s="17"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>45</v>
+      </c>
+      <c r="B3" s="17" t="str">
+        <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Corn grain</v>
+      </c>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="19">
+        <v>50</v>
+      </c>
+      <c r="B4" s="22" t="str">
+        <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Corn silage</v>
+      </c>
+      <c r="C4" s="17"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>58</v>
+      </c>
+      <c r="B5" s="17" t="str">
+        <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Cottonseed meal</v>
+      </c>
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>59</v>
+      </c>
+      <c r="B6" s="17" t="str">
+        <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Cottonseed whole</v>
+      </c>
+      <c r="C6" s="17"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>60</v>
+      </c>
+      <c r="B7" s="17" t="str">
+        <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Distillers grain plus soluble, dry</v>
+      </c>
+      <c r="C7" s="17"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
+        <v>79</v>
+      </c>
+      <c r="B8" s="17" t="str">
+        <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Grain sorghum grain</v>
+      </c>
+      <c r="C8" s="17"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
+        <v>133</v>
+      </c>
+      <c r="B9" s="17" t="str">
+        <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Soybean hulls</v>
+      </c>
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>134</v>
+      </c>
+      <c r="B10" s="17" t="str">
+        <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Soybean meal high CP</v>
+      </c>
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>148</v>
+      </c>
+      <c r="B11" s="17" t="str">
+        <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Sugarcane silage</v>
+      </c>
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
+        <v>166</v>
+      </c>
+      <c r="B12" s="17" t="str">
+        <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Wheat middlings</v>
+      </c>
+      <c r="C12" s="17"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
+        <v>845</v>
+      </c>
+      <c r="B13" s="17" t="str">
+        <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Urea</v>
+      </c>
+      <c r="C13" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="A1:BF219"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A126" workbookViewId="0">
       <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
@@ -40731,10 +41056,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:BF219">
-    <cfRule type="expression" dxfId="61" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="1" stopIfTrue="1">
       <formula>ROW(A2)=$E$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="2" stopIfTrue="1">
       <formula>COLUMN(A2)=$F$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40746,7 +41071,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A58"/>
   <sheetViews>
@@ -41055,12 +41380,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003C4402FDC8975A4FB65AB474AF423692" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="43da31f6e8d8dfaec40561525ce78865">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="871f9270-bc3b-4105-9923-e7982e1cb312" xmlns:ns4="000447b7-86fa-4362-939e-855579e16124" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b58fc7e6f492e58d10793199fba37542" ns3:_="" ns4:_="">
     <xsd:import namespace="871f9270-bc3b-4105-9923-e7982e1cb312"/>
@@ -41263,7 +41582,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -41272,24 +41591,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE8DA1A1-DD54-4881-BC06-911C3C5870BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41308,10 +41616,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Datasets, logging and name adjusted
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1896157_ed_ac_uk/Documents/Rafael/Models/GreenFeeding/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1896157\OneDrive - University of Edinburgh\Rafael\Models\GreenFeeding\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -1262,52 +1262,18 @@
   </cellStyles>
   <dxfs count="74">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="none">
+        <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="none">
+        <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1608,22 +1574,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
@@ -1694,6 +1644,56 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1708,17 +1708,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:E13" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:E13" totalsRowShown="0" dataDxfId="73">
   <autoFilter ref="A1:E13"/>
   <sortState ref="A2:E30">
     <sortCondition ref="A1:A30"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="4"/>
-    <tableColumn id="2" name="Min" dataDxfId="3"/>
-    <tableColumn id="3" name="Max" dataDxfId="2"/>
-    <tableColumn id="4" name="Cost" dataDxfId="1"/>
-    <tableColumn id="5" name="Name" dataDxfId="0">
+    <tableColumn id="1" name="ID" dataDxfId="72"/>
+    <tableColumn id="2" name="Min" dataDxfId="71"/>
+    <tableColumn id="3" name="Max" dataDxfId="70"/>
+    <tableColumn id="4" name="Cost" dataDxfId="69"/>
+    <tableColumn id="5" name="Name" dataDxfId="68">
       <calculatedColumnFormula>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1727,7 +1727,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="73" tableBorderDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="67" tableBorderDxfId="66">
   <autoFilter ref="A1:Q3"/>
   <tableColumns count="17">
     <tableColumn id="1" name="ID"/>
@@ -1770,87 +1770,87 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela26" displayName="Tabela26" ref="A1:C13" totalsRowShown="0" dataDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela26" displayName="Tabela26" ref="A1:C13" totalsRowShown="0" dataDxfId="65">
   <autoFilter ref="A1:C13"/>
   <sortState ref="A2:E30">
     <sortCondition ref="A1:A30"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="ID" dataDxfId="70"/>
-    <tableColumn id="5" name="Name" dataDxfId="69">
+    <tableColumn id="1" name="ID" dataDxfId="64"/>
+    <tableColumn id="5" name="Name" dataDxfId="63">
       <calculatedColumnFormula>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="LCA_GHG" dataDxfId="68"/>
+    <tableColumn id="6" name="LCA_GHG" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:BF219" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:BF219" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A1:BF219"/>
   <sortState ref="A2:BF219">
     <sortCondition ref="A4:A5"/>
   </sortState>
   <tableColumns count="58">
-    <tableColumn id="1" name="ID" dataDxfId="63"/>
-    <tableColumn id="2" name="Feed" dataDxfId="62"/>
-    <tableColumn id="4" name="IFN" dataDxfId="61"/>
-    <tableColumn id="5" name="Cost, $/Tonne AF" dataDxfId="60"/>
-    <tableColumn id="7" name="Forage, %DM" dataDxfId="59"/>
-    <tableColumn id="8" name="DM, %AF" dataDxfId="58"/>
-    <tableColumn id="16" name="CP, %DM" dataDxfId="57"/>
-    <tableColumn id="31" name="SP, %CP" dataDxfId="56"/>
-    <tableColumn id="29" name="ADICP, %CP" dataDxfId="55"/>
-    <tableColumn id="24" name="Sugars, %DM" dataDxfId="54"/>
-    <tableColumn id="25" name="OA, %DM" dataDxfId="53"/>
-    <tableColumn id="23" name="Fat, %DM" dataDxfId="52"/>
-    <tableColumn id="9" name="Ash, %DM" dataDxfId="51"/>
-    <tableColumn id="10" name="Starch, %DM" dataDxfId="50"/>
-    <tableColumn id="12" name="NDF, %DM" dataDxfId="49"/>
-    <tableColumn id="13" name="Lignin, %DM" dataDxfId="48"/>
-    <tableColumn id="14" name="TDN, %DM" dataDxfId="47"/>
-    <tableColumn id="15" name="ME, Mcal/kg" dataDxfId="46"/>
-    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="45"/>
-    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="44"/>
-    <tableColumn id="21" name="RUP, %CP" dataDxfId="43"/>
-    <tableColumn id="22" name="kd PB, %/h" dataDxfId="42"/>
-    <tableColumn id="26" name="kd CB1, %/h" dataDxfId="41"/>
-    <tableColumn id="27" name="kd CB2, %/h" dataDxfId="40"/>
-    <tableColumn id="17" name="kd CB3, %/h" dataDxfId="39"/>
-    <tableColumn id="28" name="PBID, %" dataDxfId="38"/>
-    <tableColumn id="6" name="CB1ID, %" dataDxfId="37"/>
-    <tableColumn id="3" name="CB2ID, %" dataDxfId="36"/>
-    <tableColumn id="20" name="pef, %NDF" dataDxfId="35"/>
-    <tableColumn id="11" name="ARG, %DM" dataDxfId="34"/>
-    <tableColumn id="32" name="HIS, %DM" dataDxfId="33"/>
-    <tableColumn id="33" name="ILE, %DM" dataDxfId="32"/>
-    <tableColumn id="34" name="LEU, %DM" dataDxfId="31"/>
-    <tableColumn id="35" name="LYS, %DM" dataDxfId="30"/>
-    <tableColumn id="36" name="MET, %DM" dataDxfId="29"/>
-    <tableColumn id="37" name="CYS, %DM" dataDxfId="28"/>
-    <tableColumn id="38" name="PHE, %DM" dataDxfId="27"/>
-    <tableColumn id="39" name="TYR, %DM" dataDxfId="26"/>
-    <tableColumn id="40" name="THR, %DM" dataDxfId="25"/>
-    <tableColumn id="41" name="TRP, %DM" dataDxfId="24"/>
-    <tableColumn id="42" name="VAL, %DM" dataDxfId="23"/>
-    <tableColumn id="43" name="Ca, % DM" dataDxfId="22"/>
-    <tableColumn id="44" name="P, % DM" dataDxfId="21"/>
-    <tableColumn id="45" name="Mg, % DM" dataDxfId="20"/>
-    <tableColumn id="46" name="Cl, % DM" dataDxfId="19"/>
-    <tableColumn id="47" name="K, % DM" dataDxfId="18"/>
-    <tableColumn id="48" name="Na, % DM" dataDxfId="17"/>
-    <tableColumn id="49" name="S, % DM" dataDxfId="16"/>
-    <tableColumn id="50" name="Co, mg/kg" dataDxfId="15"/>
-    <tableColumn id="51" name="Cu, mg/kg" dataDxfId="14"/>
-    <tableColumn id="52" name="I, mg/kg" dataDxfId="13"/>
-    <tableColumn id="53" name="Fe, mg/kg" dataDxfId="12"/>
-    <tableColumn id="54" name="Mn, mg/kg" dataDxfId="11"/>
-    <tableColumn id="55" name="Se, mg/kg" dataDxfId="10"/>
-    <tableColumn id="56" name="Zn, mg/kg" dataDxfId="9"/>
-    <tableColumn id="57" name="Vit A, IU/g" dataDxfId="8"/>
-    <tableColumn id="58" name="Vit D, IU/g" dataDxfId="7"/>
-    <tableColumn id="30" name="Vit E, IU/kg" dataDxfId="6"/>
+    <tableColumn id="1" name="ID" dataDxfId="59"/>
+    <tableColumn id="2" name="Feed" dataDxfId="58"/>
+    <tableColumn id="4" name="IFN" dataDxfId="57"/>
+    <tableColumn id="5" name="Cost, $/Tonne AF" dataDxfId="56"/>
+    <tableColumn id="7" name="Forage, %DM" dataDxfId="55"/>
+    <tableColumn id="8" name="DM, %AF" dataDxfId="54"/>
+    <tableColumn id="16" name="CP, %DM" dataDxfId="53"/>
+    <tableColumn id="31" name="SP, %CP" dataDxfId="52"/>
+    <tableColumn id="29" name="ADICP, %CP" dataDxfId="51"/>
+    <tableColumn id="24" name="Sugars, %DM" dataDxfId="50"/>
+    <tableColumn id="25" name="OA, %DM" dataDxfId="49"/>
+    <tableColumn id="23" name="Fat, %DM" dataDxfId="48"/>
+    <tableColumn id="9" name="Ash, %DM" dataDxfId="47"/>
+    <tableColumn id="10" name="Starch, %DM" dataDxfId="46"/>
+    <tableColumn id="12" name="NDF, %DM" dataDxfId="45"/>
+    <tableColumn id="13" name="Lignin, %DM" dataDxfId="44"/>
+    <tableColumn id="14" name="TDN, %DM" dataDxfId="43"/>
+    <tableColumn id="15" name="ME, Mcal/kg" dataDxfId="42"/>
+    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="41"/>
+    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="40"/>
+    <tableColumn id="21" name="RUP, %CP" dataDxfId="39"/>
+    <tableColumn id="22" name="kd PB, %/h" dataDxfId="38"/>
+    <tableColumn id="26" name="kd CB1, %/h" dataDxfId="37"/>
+    <tableColumn id="27" name="kd CB2, %/h" dataDxfId="36"/>
+    <tableColumn id="17" name="kd CB3, %/h" dataDxfId="35"/>
+    <tableColumn id="28" name="PBID, %" dataDxfId="34"/>
+    <tableColumn id="6" name="CB1ID, %" dataDxfId="33"/>
+    <tableColumn id="3" name="CB2ID, %" dataDxfId="32"/>
+    <tableColumn id="20" name="pef, %NDF" dataDxfId="31"/>
+    <tableColumn id="11" name="ARG, %DM" dataDxfId="30"/>
+    <tableColumn id="32" name="HIS, %DM" dataDxfId="29"/>
+    <tableColumn id="33" name="ILE, %DM" dataDxfId="28"/>
+    <tableColumn id="34" name="LEU, %DM" dataDxfId="27"/>
+    <tableColumn id="35" name="LYS, %DM" dataDxfId="26"/>
+    <tableColumn id="36" name="MET, %DM" dataDxfId="25"/>
+    <tableColumn id="37" name="CYS, %DM" dataDxfId="24"/>
+    <tableColumn id="38" name="PHE, %DM" dataDxfId="23"/>
+    <tableColumn id="39" name="TYR, %DM" dataDxfId="22"/>
+    <tableColumn id="40" name="THR, %DM" dataDxfId="21"/>
+    <tableColumn id="41" name="TRP, %DM" dataDxfId="20"/>
+    <tableColumn id="42" name="VAL, %DM" dataDxfId="19"/>
+    <tableColumn id="43" name="Ca, % DM" dataDxfId="18"/>
+    <tableColumn id="44" name="P, % DM" dataDxfId="17"/>
+    <tableColumn id="45" name="Mg, % DM" dataDxfId="16"/>
+    <tableColumn id="46" name="Cl, % DM" dataDxfId="15"/>
+    <tableColumn id="47" name="K, % DM" dataDxfId="14"/>
+    <tableColumn id="48" name="Na, % DM" dataDxfId="13"/>
+    <tableColumn id="49" name="S, % DM" dataDxfId="12"/>
+    <tableColumn id="50" name="Co, mg/kg" dataDxfId="11"/>
+    <tableColumn id="51" name="Cu, mg/kg" dataDxfId="10"/>
+    <tableColumn id="52" name="I, mg/kg" dataDxfId="9"/>
+    <tableColumn id="53" name="Fe, mg/kg" dataDxfId="8"/>
+    <tableColumn id="54" name="Mn, mg/kg" dataDxfId="7"/>
+    <tableColumn id="55" name="Se, mg/kg" dataDxfId="6"/>
+    <tableColumn id="56" name="Zn, mg/kg" dataDxfId="5"/>
+    <tableColumn id="57" name="Vit A, IU/g" dataDxfId="4"/>
+    <tableColumn id="58" name="Vit D, IU/g" dataDxfId="3"/>
+    <tableColumn id="30" name="Vit E, IU/kg" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2124,8 +2124,8 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2385,8 +2385,8 @@
   </sheetPr>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2561,7 +2561,7 @@
         <v>1E-3</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -2579,7 +2579,9 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="D13:E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2656,7 +2658,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2797,8 +2799,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2810,8 +2813,8 @@
   </sheetPr>
   <dimension ref="A1:BF219"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="B147" sqref="B147"/>
+    <sheetView topLeftCell="AP1" workbookViewId="0">
+      <selection sqref="A1:BF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41056,10 +41059,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:BF219">
-    <cfRule type="expression" dxfId="67" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>ROW(A2)=$E$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>COLUMN(A2)=$F$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41380,6 +41383,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003C4402FDC8975A4FB65AB474AF423692" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="43da31f6e8d8dfaec40561525ce78865">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="871f9270-bc3b-4105-9923-e7982e1cb312" xmlns:ns4="000447b7-86fa-4362-939e-855579e16124" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b58fc7e6f492e58d10793199fba37542" ns3:_="" ns4:_="">
     <xsd:import namespace="871f9270-bc3b-4105-9923-e7982e1cb312"/>
@@ -41582,15 +41594,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -41598,6 +41601,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE8DA1A1-DD54-4881-BC06-911C3C5870BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41616,24 +41627,16 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>

</xml_diff>

<commit_message>
Feed ID implemented, lca fixed
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -28,8 +28,92 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>MARQUES Gabriel</author>
+  </authors>
+  <commentList>
+    <comment ref="E18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MARQUES Gabriel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+0.11</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MARQUES Gabriel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+0.14
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MARQUES Gabriel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+0.1
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="351">
   <si>
     <t>IFN</t>
   </si>
@@ -1015,9 +1099,6 @@
     <t>Algorithm</t>
   </si>
   <si>
-    <t>GSS</t>
-  </si>
-  <si>
     <t>BF</t>
   </si>
   <si>
@@ -1036,22 +1117,13 @@
     <t>Cost</t>
   </si>
   <si>
-    <t>E-BF</t>
-  </si>
-  <si>
     <t>LCA_GHG_weight</t>
   </si>
   <si>
     <t>LCA_GHG</t>
   </si>
   <si>
-    <t>LCA_cost</t>
-  </si>
-  <si>
     <t>Epislon</t>
-  </si>
-  <si>
-    <t>LCA_weight</t>
   </si>
   <si>
     <t>Methane</t>
@@ -1063,7 +1135,37 @@
     <t>Methane_Equation</t>
   </si>
   <si>
-    <t>LCA_ID</t>
+    <t>Feed Scenario</t>
+  </si>
+  <si>
+    <t>LCA ID</t>
+  </si>
+  <si>
+    <t>Obj</t>
+  </si>
+  <si>
+    <t>MaxProfit</t>
+  </si>
+  <si>
+    <t>GSS</t>
+  </si>
+  <si>
+    <t>GSS-Max</t>
+  </si>
+  <si>
+    <t>MinCost</t>
+  </si>
+  <si>
+    <t>MaxProfitSWG</t>
+  </si>
+  <si>
+    <t>GSS-MaxSWG</t>
+  </si>
+  <si>
+    <t>LCA weight</t>
+  </si>
+  <si>
+    <t>LCA cost</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1176,7 @@
     <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
     <numFmt numFmtId="165" formatCode="0.00;0.00;0;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1089,6 +1191,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1221,7 +1343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1">
@@ -1256,11 +1378,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="74">
+  <dxfs count="76">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1606,6 +1730,39 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -1694,6 +1851,14 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1708,18 +1873,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:E13" totalsRowShown="0" dataDxfId="73">
-  <autoFilter ref="A1:E13"/>
-  <sortState ref="A2:E30">
-    <sortCondition ref="A1:A30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F24" totalsRowShown="0" dataDxfId="75">
+  <autoFilter ref="A1:F24"/>
+  <sortState ref="B2:F30">
+    <sortCondition ref="B1:B30"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="72"/>
-    <tableColumn id="2" name="Min" dataDxfId="71"/>
-    <tableColumn id="3" name="Max" dataDxfId="70"/>
-    <tableColumn id="4" name="Cost" dataDxfId="69"/>
-    <tableColumn id="5" name="Name" dataDxfId="68">
-      <calculatedColumnFormula>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</calculatedColumnFormula>
+  <tableColumns count="6">
+    <tableColumn id="6" name="Feed Scenario" dataDxfId="74"/>
+    <tableColumn id="1" name="ID" dataDxfId="73"/>
+    <tableColumn id="2" name="Min" dataDxfId="72"/>
+    <tableColumn id="3" name="Max" dataDxfId="71"/>
+    <tableColumn id="4" name="Cost" dataDxfId="70"/>
+    <tableColumn id="5" name="Name" dataDxfId="69">
+      <calculatedColumnFormula>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1727,10 +1893,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="67" tableBorderDxfId="66">
-  <autoFilter ref="A1:Q3"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:S4" totalsRowShown="0" headerRowDxfId="68" tableBorderDxfId="67">
+  <autoFilter ref="A1:S4"/>
+  <tableColumns count="19">
     <tableColumn id="1" name="ID"/>
+    <tableColumn id="18" name="Feed Scenario" dataDxfId="66"/>
     <tableColumn id="2" name="Breed"/>
     <tableColumn id="3" name="SBW"/>
     <tableColumn id="4" name="BCS"/>
@@ -1746,21 +1913,21 @@
     <tableColumn id="14" name="LB"/>
     <tableColumn id="15" name="UB"/>
     <tableColumn id="16" name="Tol"/>
-    <tableColumn id="17" name="LCA_ID"/>
+    <tableColumn id="17" name="LCA ID"/>
+    <tableColumn id="19" name="Obj"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:H2" totalsRowShown="0">
-  <autoFilter ref="A1:H2"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G3" totalsRowShown="0">
+  <autoFilter ref="A1:G3"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="LCA_cost"/>
+    <tableColumn id="2" name="LCA cost"/>
     <tableColumn id="3" name="Epislon"/>
-    <tableColumn id="4" name="LCA_weight"/>
-    <tableColumn id="5" name="LCA_GHG"/>
+    <tableColumn id="4" name="LCA weight"/>
     <tableColumn id="6" name="LCA_GHG_weight"/>
     <tableColumn id="7" name="Methane"/>
     <tableColumn id="8" name="Methane_Equation"/>
@@ -1770,8 +1937,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela26" displayName="Tabela26" ref="A1:C13" totalsRowShown="0" dataDxfId="65">
-  <autoFilter ref="A1:C13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela26" displayName="Tabela26" ref="A1:C14" totalsRowShown="0" dataDxfId="65">
+  <autoFilter ref="A1:C14"/>
   <sortState ref="A2:E30">
     <sortCondition ref="A1:A30"/>
   </sortState>
@@ -2118,14 +2285,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,243 +2304,514 @@
     <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>313</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>314</v>
       </c>
-      <c r="D1" t="s">
-        <v>334</v>
-      </c>
       <c r="E1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16">
         <v>34</v>
       </c>
-      <c r="B2" s="17">
-        <v>0</v>
-      </c>
       <c r="C2" s="17">
+        <v>0</v>
+      </c>
+      <c r="D2" s="17">
         <v>20</v>
       </c>
-      <c r="D2" s="18">
+      <c r="E2" s="18">
         <v>0.13888888888888887</v>
       </c>
-      <c r="E2" s="17" t="str">
-        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+      <c r="F2" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
         <v>Citrus pulp, dry</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16">
         <v>45</v>
       </c>
-      <c r="B3" s="17">
-        <v>0</v>
-      </c>
       <c r="C3" s="17">
+        <v>0</v>
+      </c>
+      <c r="D3" s="17">
         <v>20</v>
       </c>
-      <c r="D3" s="18">
+      <c r="E3" s="18">
         <v>0.17676767676767677</v>
       </c>
-      <c r="E3" s="17" t="str">
-        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+      <c r="F3" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
         <v>Corn grain</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>1</v>
+      </c>
+      <c r="B4" s="19">
         <v>50</v>
       </c>
-      <c r="B4" s="20">
-        <v>0</v>
-      </c>
       <c r="C4" s="20">
+        <v>0</v>
+      </c>
+      <c r="D4" s="20">
         <v>20</v>
       </c>
-      <c r="D4" s="21">
+      <c r="E4" s="21">
         <v>0.19</v>
       </c>
-      <c r="E4" s="22" t="str">
-        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+      <c r="F4" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
         <v>Corn silage</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>1</v>
+      </c>
+      <c r="B5" s="17">
         <v>58</v>
       </c>
-      <c r="B5" s="17">
-        <v>0</v>
-      </c>
       <c r="C5" s="17">
+        <v>0</v>
+      </c>
+      <c r="D5" s="17">
         <v>20</v>
       </c>
-      <c r="D5" s="18">
+      <c r="E5" s="18">
         <v>0.33333333333333337</v>
       </c>
-      <c r="E5" s="17" t="str">
-        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+      <c r="F5" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
         <v>Cottonseed meal</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <v>1</v>
+      </c>
+      <c r="B6" s="17">
         <v>59</v>
       </c>
-      <c r="B6" s="17">
-        <v>0</v>
-      </c>
       <c r="C6" s="17">
+        <v>0</v>
+      </c>
+      <c r="D6" s="17">
         <v>20</v>
       </c>
-      <c r="D6" s="18">
+      <c r="E6" s="18">
         <v>0.11363636363636365</v>
       </c>
-      <c r="E6" s="17" t="str">
-        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+      <c r="F6" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
         <v>Cottonseed whole</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>1</v>
+      </c>
+      <c r="B7" s="17">
         <v>60</v>
       </c>
-      <c r="B7" s="17">
-        <v>0</v>
-      </c>
       <c r="C7" s="17">
+        <v>0</v>
+      </c>
+      <c r="D7" s="17">
         <v>20</v>
       </c>
-      <c r="D7" s="18">
+      <c r="E7" s="18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E7" s="17" t="str">
-        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+      <c r="F7" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
         <v>Distillers grain plus soluble, dry</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>1</v>
+      </c>
+      <c r="B8" s="17">
         <v>79</v>
       </c>
-      <c r="B8" s="17">
-        <v>0</v>
-      </c>
       <c r="C8" s="17">
+        <v>0</v>
+      </c>
+      <c r="D8" s="17">
         <v>20</v>
       </c>
-      <c r="D8" s="18">
+      <c r="E8" s="18">
         <v>0.10101010101010102</v>
       </c>
-      <c r="E8" s="17" t="str">
-        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+      <c r="F8" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
         <v>Grain sorghum grain</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>1</v>
+      </c>
+      <c r="B9" s="17">
         <v>133</v>
       </c>
-      <c r="B9" s="17">
-        <v>0</v>
-      </c>
       <c r="C9" s="17">
+        <v>0</v>
+      </c>
+      <c r="D9" s="17">
         <v>20</v>
       </c>
-      <c r="D9" s="18">
+      <c r="E9" s="18">
         <v>0.16414141414141412</v>
       </c>
-      <c r="E9" s="17" t="str">
-        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+      <c r="F9" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
         <v>Soybean hulls</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>1</v>
+      </c>
+      <c r="B10" s="17">
         <v>134</v>
       </c>
-      <c r="B10" s="17">
-        <v>0</v>
-      </c>
       <c r="C10" s="17">
+        <v>0</v>
+      </c>
+      <c r="D10" s="17">
         <v>20</v>
       </c>
-      <c r="D10" s="18">
+      <c r="E10" s="18">
         <v>0.19696969696969696</v>
       </c>
-      <c r="E10" s="17" t="str">
-        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+      <c r="F10" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
         <v>Soybean meal high CP</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>1</v>
+      </c>
+      <c r="B11" s="17">
         <v>148</v>
       </c>
-      <c r="B11" s="17">
-        <v>0</v>
-      </c>
       <c r="C11" s="17">
+        <v>0</v>
+      </c>
+      <c r="D11" s="17">
         <v>20</v>
       </c>
-      <c r="D11" s="18">
+      <c r="E11" s="18">
         <v>8.8383838383838384E-2</v>
       </c>
-      <c r="E11" s="17" t="str">
-        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+      <c r="F11" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
         <v>Sugarcane silage</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>1</v>
+      </c>
+      <c r="B12" s="17">
         <v>166</v>
       </c>
-      <c r="B12" s="17">
-        <v>0</v>
-      </c>
       <c r="C12" s="17">
+        <v>0</v>
+      </c>
+      <c r="D12" s="17">
         <v>20</v>
       </c>
-      <c r="D12" s="18">
+      <c r="E12" s="18">
         <v>0.15151515151515152</v>
       </c>
-      <c r="E12" s="17" t="str">
-        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+      <c r="F12" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
         <v>Wheat middlings</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
+        <v>1</v>
+      </c>
+      <c r="B13" s="16">
         <v>845</v>
       </c>
-      <c r="B13" s="17">
-        <v>0</v>
-      </c>
       <c r="C13" s="17">
+        <v>0</v>
+      </c>
+      <c r="D13" s="17">
         <v>20</v>
       </c>
-      <c r="D13" s="18">
+      <c r="E13" s="18">
         <v>0.40404040404040409</v>
       </c>
-      <c r="E13" s="17" t="str">
-        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+      <c r="F13" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
+        <v>Urea</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <v>2</v>
+      </c>
+      <c r="B14" s="16">
+        <v>1</v>
+      </c>
+      <c r="C14" s="17">
+        <v>0</v>
+      </c>
+      <c r="D14" s="17">
+        <v>1</v>
+      </c>
+      <c r="E14" s="18">
+        <v>6</v>
+      </c>
+      <c r="F14" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
+        <v>Alfalfa cubes</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
+        <v>2</v>
+      </c>
+      <c r="B15" s="16">
+        <v>34</v>
+      </c>
+      <c r="C15" s="17">
+        <v>0</v>
+      </c>
+      <c r="D15" s="17">
+        <v>1</v>
+      </c>
+      <c r="E15" s="18">
+        <v>0.19</v>
+      </c>
+      <c r="F15" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
+        <v>Citrus pulp, dry</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="17">
+        <v>2</v>
+      </c>
+      <c r="B16" s="16">
+        <v>45</v>
+      </c>
+      <c r="C16" s="17">
+        <v>0</v>
+      </c>
+      <c r="D16" s="17">
+        <v>1</v>
+      </c>
+      <c r="E16" s="18">
+        <v>0.15</v>
+      </c>
+      <c r="F16" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
+        <v>Corn grain</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
+        <v>2</v>
+      </c>
+      <c r="B17" s="16">
+        <v>50</v>
+      </c>
+      <c r="C17" s="17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="18">
+        <v>0.19</v>
+      </c>
+      <c r="F17" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
+        <v>Corn silage</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>2</v>
+      </c>
+      <c r="B18" s="17">
+        <v>59</v>
+      </c>
+      <c r="C18" s="17">
+        <v>0</v>
+      </c>
+      <c r="D18" s="17">
+        <v>1</v>
+      </c>
+      <c r="E18" s="18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F18" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
+        <v>Cottonseed whole</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>2</v>
+      </c>
+      <c r="B19" s="17">
+        <v>60</v>
+      </c>
+      <c r="C19" s="17">
+        <v>0</v>
+      </c>
+      <c r="D19" s="17">
+        <v>1</v>
+      </c>
+      <c r="E19" s="18">
+        <v>0.08</v>
+      </c>
+      <c r="F19" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
+        <v>Distillers grain plus soluble, dry</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>2</v>
+      </c>
+      <c r="B20" s="17">
+        <v>79</v>
+      </c>
+      <c r="C20" s="17">
+        <v>0</v>
+      </c>
+      <c r="D20" s="17">
+        <v>1</v>
+      </c>
+      <c r="E20" s="18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F20" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
+        <v>Grain sorghum grain</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
+        <v>2</v>
+      </c>
+      <c r="B21" s="17">
+        <v>133</v>
+      </c>
+      <c r="C21" s="17">
+        <v>0</v>
+      </c>
+      <c r="D21" s="17">
+        <v>1</v>
+      </c>
+      <c r="E21" s="18">
+        <v>0.16414141414141412</v>
+      </c>
+      <c r="F21" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
+        <v>Soybean hulls</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="17">
+        <v>2</v>
+      </c>
+      <c r="B22" s="17">
+        <v>134</v>
+      </c>
+      <c r="C22" s="17">
+        <v>0</v>
+      </c>
+      <c r="D22" s="17">
+        <v>1</v>
+      </c>
+      <c r="E22" s="18">
+        <v>0.19696969696969696</v>
+      </c>
+      <c r="F22" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
+        <v>Soybean meal high CP</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
+        <v>2</v>
+      </c>
+      <c r="B23" s="17">
+        <v>148</v>
+      </c>
+      <c r="C23" s="17">
+        <v>0</v>
+      </c>
+      <c r="D23" s="17">
+        <v>1</v>
+      </c>
+      <c r="E23" s="18">
+        <v>0.15151515151515152</v>
+      </c>
+      <c r="F23" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
+        <v>Sugarcane silage</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="17">
+        <v>2</v>
+      </c>
+      <c r="B24" s="16">
+        <v>845</v>
+      </c>
+      <c r="C24" s="17">
+        <v>0</v>
+      </c>
+      <c r="D24" s="17">
+        <v>1</v>
+      </c>
+      <c r="E24" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="F24" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
         <v>Urea</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2383,96 +2821,103 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>319</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>320</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="H1" s="26" t="s">
         <v>321</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="I1" s="26" t="s">
         <v>322</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="J1" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>324</v>
       </c>
-      <c r="K1" s="27" t="s">
-        <v>333</v>
-      </c>
-      <c r="L1" s="28" t="s">
+      <c r="L1" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="M1" s="28" t="s">
         <v>327</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="N1" s="28" t="s">
         <v>326</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="O1" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="P1" s="28" t="s">
         <v>330</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="Q1" s="28" t="s">
         <v>331</v>
       </c>
-      <c r="P1" s="28" t="s">
-        <v>332</v>
-      </c>
-      <c r="Q1" s="29" t="s">
-        <v>344</v>
+      <c r="R1" s="29" t="s">
+        <v>341</v>
+      </c>
+      <c r="S1" s="29" t="s">
+        <v>342</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>318</v>
       </c>
-      <c r="C2" s="24">
+      <c r="D2" s="24">
         <v>300</v>
       </c>
-      <c r="D2" s="24">
+      <c r="E2" s="24">
         <v>5</v>
-      </c>
-      <c r="E2" s="24">
-        <v>1</v>
       </c>
       <c r="F2" s="24">
         <v>1</v>
@@ -2481,51 +2926,57 @@
         <v>1</v>
       </c>
       <c r="H2" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="24">
+        <v>0</v>
+      </c>
+      <c r="J2" s="24">
         <v>6.2</v>
       </c>
-      <c r="J2" s="24">
+      <c r="K2" s="24">
         <v>1.44</v>
       </c>
-      <c r="K2" s="25">
-        <v>13.91</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>328</v>
+      <c r="L2" s="25">
+        <v>0.87</v>
       </c>
       <c r="M2" s="23" t="s">
         <v>328</v>
       </c>
-      <c r="N2" s="23">
+      <c r="N2" s="23" t="s">
+        <v>328</v>
+      </c>
+      <c r="O2" s="23">
         <v>0.8</v>
       </c>
-      <c r="O2" s="23">
-        <v>3</v>
-      </c>
       <c r="P2" s="23">
-        <v>1E-3</v>
+        <v>2</v>
       </c>
       <c r="Q2">
-        <v>-1</v>
+        <v>0.01</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>343</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="30">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>318</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>300</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>5</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2534,34 +2985,99 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>6.2</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>1.44</v>
       </c>
-      <c r="K3">
-        <v>13.91</v>
-      </c>
-      <c r="L3" t="s">
-        <v>329</v>
+      <c r="L3">
+        <v>0.87</v>
       </c>
       <c r="M3" t="s">
-        <v>335</v>
-      </c>
-      <c r="N3">
+        <v>344</v>
+      </c>
+      <c r="N3" t="s">
+        <v>345</v>
+      </c>
+      <c r="O3">
         <v>0.8</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>3</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>1E-3</v>
       </c>
-      <c r="Q3">
-        <v>-1</v>
+      <c r="R3">
+        <v>2</v>
+      </c>
+      <c r="S3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="30">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D4">
+        <v>300</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>6.2</v>
+      </c>
+      <c r="K4">
+        <v>1.44</v>
+      </c>
+      <c r="L4">
+        <v>0.87</v>
+      </c>
+      <c r="M4" t="s">
+        <v>344</v>
+      </c>
+      <c r="N4" t="s">
+        <v>348</v>
+      </c>
+      <c r="O4">
+        <v>0.8</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <v>1E-3</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -2577,10 +3093,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="D13:E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2588,57 +3104,70 @@
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>338</v>
+        <v>350</v>
       </c>
       <c r="C1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G1" t="s">
         <v>339</v>
       </c>
-      <c r="D1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E1" t="s">
-        <v>337</v>
-      </c>
-      <c r="F1" t="s">
-        <v>336</v>
-      </c>
-      <c r="G1" t="s">
-        <v>341</v>
-      </c>
-      <c r="H1" t="s">
-        <v>343</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.05</v>
+        <v>5.0000000000000004E-6</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" t="b">
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="G2" t="b">
+      <c r="G2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="b">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>342</v>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -2655,10 +3184,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2674,128 +3203,164 @@
         <v>325</v>
       </c>
       <c r="C1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
-        <v>34</v>
-      </c>
-      <c r="B2" s="17" t="str">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="31" t="str">
         <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
-        <v>Citrus pulp, dry</v>
-      </c>
-      <c r="C2" s="17"/>
+        <v>Alfalfa cubes</v>
+      </c>
+      <c r="C2" s="17">
+        <v>666</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B3" s="17" t="str">
         <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
-        <v>Corn grain</v>
-      </c>
-      <c r="C3" s="17"/>
+        <v>Citrus pulp, dry</v>
+      </c>
+      <c r="C3" s="17">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+      <c r="A4" s="16">
+        <v>45</v>
+      </c>
+      <c r="B4" s="17" t="str">
+        <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Corn grain</v>
+      </c>
+      <c r="C4" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="19">
         <v>50</v>
       </c>
-      <c r="B4" s="22" t="str">
+      <c r="B5" s="22" t="str">
         <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
         <v>Corn silage</v>
       </c>
-      <c r="C4" s="17"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
-        <v>58</v>
-      </c>
-      <c r="B5" s="17" t="str">
-        <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
-        <v>Cottonseed meal</v>
-      </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="17">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="17" t="str">
         <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
-        <v>Cottonseed whole</v>
-      </c>
-      <c r="C6" s="17"/>
+        <v>Cottonseed meal</v>
+      </c>
+      <c r="C6" s="17">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="17" t="str">
         <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
-        <v>Distillers grain plus soluble, dry</v>
-      </c>
-      <c r="C7" s="17"/>
+        <v>Cottonseed whole</v>
+      </c>
+      <c r="C7" s="17">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B8" s="17" t="str">
         <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
-        <v>Grain sorghum grain</v>
-      </c>
-      <c r="C8" s="17"/>
+        <v>Distillers grain plus soluble, dry</v>
+      </c>
+      <c r="C8" s="17">
+        <v>44</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="B9" s="17" t="str">
         <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
-        <v>Soybean hulls</v>
-      </c>
-      <c r="C9" s="17"/>
+        <v>Grain sorghum grain</v>
+      </c>
+      <c r="C9" s="17">
+        <v>54</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10" s="17" t="str">
         <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
-        <v>Soybean meal high CP</v>
-      </c>
-      <c r="C10" s="17"/>
+        <v>Soybean hulls</v>
+      </c>
+      <c r="C10" s="17">
+        <v>66</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="B11" s="17" t="str">
         <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
-        <v>Sugarcane silage</v>
-      </c>
-      <c r="C11" s="17"/>
+        <v>Soybean meal high CP</v>
+      </c>
+      <c r="C11" s="17">
+        <v>78</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="B12" s="17" t="str">
         <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
-        <v>Wheat middlings</v>
-      </c>
-      <c r="C12" s="17"/>
+        <v>Sugarcane silage</v>
+      </c>
+      <c r="C12" s="17">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
-        <v>845</v>
+      <c r="A13" s="17">
+        <v>166</v>
       </c>
       <c r="B13" s="17" t="str">
         <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Wheat middlings</v>
+      </c>
+      <c r="C13" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <v>845</v>
+      </c>
+      <c r="B14" s="17" t="str">
+        <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
         <v>Urea</v>
       </c>
-      <c r="C13" s="17"/>
+      <c r="C14" s="17">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41383,6 +41948,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -41391,7 +41962,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003C4402FDC8975A4FB65AB474AF423692" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="43da31f6e8d8dfaec40561525ce78865">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="871f9270-bc3b-4105-9923-e7982e1cb312" xmlns:ns4="000447b7-86fa-4362-939e-855579e16124" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b58fc7e6f492e58d10793199fba37542" ns3:_="" ns4:_="">
     <xsd:import namespace="871f9270-bc3b-4105-9923-e7982e1cb312"/>
@@ -41594,13 +42165,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -41608,7 +42190,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE8DA1A1-DD54-4881-BC06-911C3C5870BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41625,21 +42207,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
-    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
multi-objective runnig for CPLEX, problems with HiGHS
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="349">
   <si>
     <t>IFN</t>
   </si>
@@ -1153,6 +1153,9 @@
     <t>Multiobjective</t>
   </si>
   <si>
+    <t>GSS</t>
+  </si>
+  <si>
     <t>MO-GSS</t>
   </si>
   <si>
@@ -1318,22 +1321,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="76">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1631,6 +1618,22 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
@@ -1872,8 +1875,8 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela26" displayName="Tabela26" ref="A1:C15" totalsRowShown="0" dataDxfId="65">
   <autoFilter ref="A1:C15"/>
-  <sortState ref="A2:E30">
-    <sortCondition ref="A1:A30"/>
+  <sortState ref="A2:C15">
+    <sortCondition ref="A1:A15"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="ID" dataDxfId="64"/>
@@ -1887,70 +1890,70 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:BF219" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:BF219" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="A1:BF219"/>
   <sortState ref="A2:BF219">
     <sortCondition ref="A4:A5"/>
   </sortState>
   <tableColumns count="58">
-    <tableColumn id="1" name="ID" dataDxfId="59"/>
-    <tableColumn id="2" name="Feed" dataDxfId="58"/>
-    <tableColumn id="4" name="IFN" dataDxfId="57"/>
-    <tableColumn id="5" name="Cost, $/Tonne AF" dataDxfId="56"/>
-    <tableColumn id="7" name="Forage, %DM" dataDxfId="55"/>
-    <tableColumn id="8" name="DM, %AF" dataDxfId="54"/>
-    <tableColumn id="16" name="CP, %DM" dataDxfId="53"/>
-    <tableColumn id="31" name="SP, %CP" dataDxfId="52"/>
-    <tableColumn id="29" name="ADICP, %CP" dataDxfId="51"/>
-    <tableColumn id="24" name="Sugars, %DM" dataDxfId="50"/>
-    <tableColumn id="25" name="OA, %DM" dataDxfId="49"/>
-    <tableColumn id="23" name="Fat, %DM" dataDxfId="48"/>
-    <tableColumn id="9" name="Ash, %DM" dataDxfId="47"/>
-    <tableColumn id="10" name="Starch, %DM" dataDxfId="46"/>
-    <tableColumn id="12" name="NDF, %DM" dataDxfId="45"/>
-    <tableColumn id="13" name="Lignin, %DM" dataDxfId="44"/>
-    <tableColumn id="14" name="TDN, %DM" dataDxfId="43"/>
-    <tableColumn id="15" name="ME, Mcal/kg" dataDxfId="42"/>
-    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="41"/>
-    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="40"/>
-    <tableColumn id="21" name="RUP, %CP" dataDxfId="39"/>
-    <tableColumn id="22" name="kd PB, %/h" dataDxfId="38"/>
-    <tableColumn id="26" name="kd CB1, %/h" dataDxfId="37"/>
-    <tableColumn id="27" name="kd CB2, %/h" dataDxfId="36"/>
-    <tableColumn id="17" name="kd CB3, %/h" dataDxfId="35"/>
-    <tableColumn id="28" name="PBID, %" dataDxfId="34"/>
-    <tableColumn id="6" name="CB1ID, %" dataDxfId="33"/>
-    <tableColumn id="3" name="CB2ID, %" dataDxfId="32"/>
-    <tableColumn id="20" name="pef, %NDF" dataDxfId="31"/>
-    <tableColumn id="11" name="ARG, %DM" dataDxfId="30"/>
-    <tableColumn id="32" name="HIS, %DM" dataDxfId="29"/>
-    <tableColumn id="33" name="ILE, %DM" dataDxfId="28"/>
-    <tableColumn id="34" name="LEU, %DM" dataDxfId="27"/>
-    <tableColumn id="35" name="LYS, %DM" dataDxfId="26"/>
-    <tableColumn id="36" name="MET, %DM" dataDxfId="25"/>
-    <tableColumn id="37" name="CYS, %DM" dataDxfId="24"/>
-    <tableColumn id="38" name="PHE, %DM" dataDxfId="23"/>
-    <tableColumn id="39" name="TYR, %DM" dataDxfId="22"/>
-    <tableColumn id="40" name="THR, %DM" dataDxfId="21"/>
-    <tableColumn id="41" name="TRP, %DM" dataDxfId="20"/>
-    <tableColumn id="42" name="VAL, %DM" dataDxfId="19"/>
-    <tableColumn id="43" name="Ca, % DM" dataDxfId="18"/>
-    <tableColumn id="44" name="P, % DM" dataDxfId="17"/>
-    <tableColumn id="45" name="Mg, % DM" dataDxfId="16"/>
-    <tableColumn id="46" name="Cl, % DM" dataDxfId="15"/>
-    <tableColumn id="47" name="K, % DM" dataDxfId="14"/>
-    <tableColumn id="48" name="Na, % DM" dataDxfId="13"/>
-    <tableColumn id="49" name="S, % DM" dataDxfId="12"/>
-    <tableColumn id="50" name="Co, mg/kg" dataDxfId="11"/>
-    <tableColumn id="51" name="Cu, mg/kg" dataDxfId="10"/>
-    <tableColumn id="52" name="I, mg/kg" dataDxfId="9"/>
-    <tableColumn id="53" name="Fe, mg/kg" dataDxfId="8"/>
-    <tableColumn id="54" name="Mn, mg/kg" dataDxfId="7"/>
-    <tableColumn id="55" name="Se, mg/kg" dataDxfId="6"/>
-    <tableColumn id="56" name="Zn, mg/kg" dataDxfId="5"/>
-    <tableColumn id="57" name="Vit A, IU/g" dataDxfId="4"/>
-    <tableColumn id="58" name="Vit D, IU/g" dataDxfId="3"/>
-    <tableColumn id="30" name="Vit E, IU/kg" dataDxfId="2"/>
+    <tableColumn id="1" name="ID" dataDxfId="57"/>
+    <tableColumn id="2" name="Feed" dataDxfId="56"/>
+    <tableColumn id="4" name="IFN" dataDxfId="55"/>
+    <tableColumn id="5" name="Cost, $/Tonne AF" dataDxfId="54"/>
+    <tableColumn id="7" name="Forage, %DM" dataDxfId="53"/>
+    <tableColumn id="8" name="DM, %AF" dataDxfId="52"/>
+    <tableColumn id="16" name="CP, %DM" dataDxfId="51"/>
+    <tableColumn id="31" name="SP, %CP" dataDxfId="50"/>
+    <tableColumn id="29" name="ADICP, %CP" dataDxfId="49"/>
+    <tableColumn id="24" name="Sugars, %DM" dataDxfId="48"/>
+    <tableColumn id="25" name="OA, %DM" dataDxfId="47"/>
+    <tableColumn id="23" name="Fat, %DM" dataDxfId="46"/>
+    <tableColumn id="9" name="Ash, %DM" dataDxfId="45"/>
+    <tableColumn id="10" name="Starch, %DM" dataDxfId="44"/>
+    <tableColumn id="12" name="NDF, %DM" dataDxfId="43"/>
+    <tableColumn id="13" name="Lignin, %DM" dataDxfId="42"/>
+    <tableColumn id="14" name="TDN, %DM" dataDxfId="41"/>
+    <tableColumn id="15" name="ME, Mcal/kg" dataDxfId="40"/>
+    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="39"/>
+    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="38"/>
+    <tableColumn id="21" name="RUP, %CP" dataDxfId="37"/>
+    <tableColumn id="22" name="kd PB, %/h" dataDxfId="36"/>
+    <tableColumn id="26" name="kd CB1, %/h" dataDxfId="35"/>
+    <tableColumn id="27" name="kd CB2, %/h" dataDxfId="34"/>
+    <tableColumn id="17" name="kd CB3, %/h" dataDxfId="33"/>
+    <tableColumn id="28" name="PBID, %" dataDxfId="32"/>
+    <tableColumn id="6" name="CB1ID, %" dataDxfId="31"/>
+    <tableColumn id="3" name="CB2ID, %" dataDxfId="30"/>
+    <tableColumn id="20" name="pef, %NDF" dataDxfId="29"/>
+    <tableColumn id="11" name="ARG, %DM" dataDxfId="28"/>
+    <tableColumn id="32" name="HIS, %DM" dataDxfId="27"/>
+    <tableColumn id="33" name="ILE, %DM" dataDxfId="26"/>
+    <tableColumn id="34" name="LEU, %DM" dataDxfId="25"/>
+    <tableColumn id="35" name="LYS, %DM" dataDxfId="24"/>
+    <tableColumn id="36" name="MET, %DM" dataDxfId="23"/>
+    <tableColumn id="37" name="CYS, %DM" dataDxfId="22"/>
+    <tableColumn id="38" name="PHE, %DM" dataDxfId="21"/>
+    <tableColumn id="39" name="TYR, %DM" dataDxfId="20"/>
+    <tableColumn id="40" name="THR, %DM" dataDxfId="19"/>
+    <tableColumn id="41" name="TRP, %DM" dataDxfId="18"/>
+    <tableColumn id="42" name="VAL, %DM" dataDxfId="17"/>
+    <tableColumn id="43" name="Ca, % DM" dataDxfId="16"/>
+    <tableColumn id="44" name="P, % DM" dataDxfId="15"/>
+    <tableColumn id="45" name="Mg, % DM" dataDxfId="14"/>
+    <tableColumn id="46" name="Cl, % DM" dataDxfId="13"/>
+    <tableColumn id="47" name="K, % DM" dataDxfId="12"/>
+    <tableColumn id="48" name="Na, % DM" dataDxfId="11"/>
+    <tableColumn id="49" name="S, % DM" dataDxfId="10"/>
+    <tableColumn id="50" name="Co, mg/kg" dataDxfId="9"/>
+    <tableColumn id="51" name="Cu, mg/kg" dataDxfId="8"/>
+    <tableColumn id="52" name="I, mg/kg" dataDxfId="7"/>
+    <tableColumn id="53" name="Fe, mg/kg" dataDxfId="6"/>
+    <tableColumn id="54" name="Mn, mg/kg" dataDxfId="5"/>
+    <tableColumn id="55" name="Se, mg/kg" dataDxfId="4"/>
+    <tableColumn id="56" name="Zn, mg/kg" dataDxfId="3"/>
+    <tableColumn id="57" name="Vit A, IU/g" dataDxfId="2"/>
+    <tableColumn id="58" name="Vit D, IU/g" dataDxfId="1"/>
+    <tableColumn id="30" name="Vit E, IU/kg" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2799,7 +2802,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2919,10 +2922,10 @@
         <v>0.87</v>
       </c>
       <c r="M2" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="N2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="O2">
         <v>1.3</v>
@@ -2931,7 +2934,7 @@
         <v>1.9550000000000001</v>
       </c>
       <c r="Q2">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="R2">
         <v>1</v>
@@ -2984,7 +2987,7 @@
         <v>341</v>
       </c>
       <c r="N3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="O3">
         <v>1.3</v>
@@ -3021,7 +3024,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="F17:I21"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3056,7 +3059,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5.0000000000000004E-6</v>
+        <v>0.05</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3074,6 +3077,9 @@
       </c>
       <c r="B3">
         <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3102,7 +3108,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3131,7 +3137,7 @@
         <v>Alfalfa cubes</v>
       </c>
       <c r="C2" s="17">
-        <v>666</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3183,39 +3189,39 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
-        <v>845</v>
+      <c r="A7" s="17">
+        <v>59</v>
       </c>
       <c r="B7" s="17" t="str">
         <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
-        <v>Urea</v>
+        <v>Cottonseed whole</v>
       </c>
       <c r="C7" s="17">
-        <v>50</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B8" s="17" t="str">
         <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
-        <v>Cottonseed whole</v>
+        <v>Distillers grain plus soluble, dry</v>
       </c>
       <c r="C8" s="17">
-        <v>11</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
-        <v>60</v>
-      </c>
-      <c r="B9" s="17" t="str">
+        <v>77</v>
+      </c>
+      <c r="B9" s="23" t="str">
         <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
-        <v>Distillers grain plus soluble, dry</v>
+        <v>Fresh soybean forage</v>
       </c>
       <c r="C9" s="17">
-        <v>44</v>
+        <v>999</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3279,15 +3285,15 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
-        <v>77</v>
-      </c>
-      <c r="B15" s="23" t="str">
+      <c r="A15" s="16">
+        <v>845</v>
+      </c>
+      <c r="B15" s="17" t="str">
         <f>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
-        <v>Fresh soybean forage</v>
+        <v>Urea</v>
       </c>
       <c r="C15" s="17">
-        <v>999</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -41552,10 +41558,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:BF219">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="1" stopIfTrue="1">
       <formula>ROW(A2)=$E$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="2" stopIfTrue="1">
       <formula>COLUMN(A2)=$F$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41876,21 +41882,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003C4402FDC8975A4FB65AB474AF423692" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="293b87d96ae3165967deaddc9dd3a283">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="871f9270-bc3b-4105-9923-e7982e1cb312" xmlns:ns4="000447b7-86fa-4362-939e-855579e16124" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="23a07973a4b986d214a26a52ed717842" ns3:_="" ns4:_="">
     <xsd:import namespace="871f9270-bc3b-4105-9923-e7982e1cb312"/>
@@ -42107,32 +42098,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C172DDCE-6A5B-4F5B-846C-532884D79266}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42149,4 +42130,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixes in the calculations and implementation of N2O emissions
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="125">
   <si>
     <t>IFN</t>
   </si>
@@ -259,9 +259,6 @@
     <t>Tol</t>
   </si>
   <si>
-    <t>Linearization factor</t>
-  </si>
-  <si>
     <t>Methane</t>
   </si>
   <si>
@@ -391,22 +388,22 @@
     <t>UREA</t>
   </si>
   <si>
-    <t xml:space="preserve">Limousin </t>
-  </si>
-  <si>
-    <t>GSS</t>
-  </si>
-  <si>
     <t>Normalize</t>
   </si>
   <si>
-    <t>GSS-MAX_CO2</t>
-  </si>
-  <si>
-    <t>GSS-MAX_BALANCED</t>
-  </si>
-  <si>
-    <t>GSS-MAX_BALANCED_N</t>
+    <t>Baled grass, temporary meadow, with clover, Northwestern region, at farm/FR S</t>
+  </si>
+  <si>
+    <t>Grass silage, horizontal silo, temporary meadow, with clover, Northwestern region, at farm/FR S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charolais </t>
+  </si>
+  <si>
+    <t>BF</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -416,7 +413,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +445,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F497D"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -528,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
@@ -585,6 +589,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1010,9 +1022,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:V4" totalsRowShown="0">
-  <autoFilter ref="A1:V4"/>
-  <tableColumns count="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:U2" totalsRowShown="0">
+  <autoFilter ref="A1:U2"/>
+  <tableColumns count="21">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Feed Scenario"/>
     <tableColumn id="3" name="Breed"/>
@@ -1026,7 +1038,6 @@
     <tableColumn id="11" name="a2"/>
     <tableColumn id="12" name="PH"/>
     <tableColumn id="13" name="Selling Price"/>
-    <tableColumn id="14" name="Linearization factor"/>
     <tableColumn id="15" name="Algorithm"/>
     <tableColumn id="16" name="Identifier"/>
     <tableColumn id="17" name="LB"/>
@@ -1041,8 +1052,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F21" totalsRowShown="0" dataDxfId="49">
-  <autoFilter ref="A1:F21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F22" totalsRowShown="0" dataDxfId="49">
+  <autoFilter ref="A1:F22"/>
   <sortState ref="B2:F30">
     <sortCondition ref="B1:B30"/>
   </sortState>
@@ -1061,8 +1072,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:K4" totalsRowShown="0">
-  <autoFilter ref="A1:K4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:K5" totalsRowShown="0">
+  <autoFilter ref="A1:K5"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="4" name="LCA weight"/>
@@ -1081,8 +1092,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela26" displayName="Tabela26" ref="A1:H21" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A1:H21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela26" displayName="Tabela26" ref="A1:H23" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A1:H23"/>
   <sortState ref="A2:C15">
     <sortCondition ref="A1:A15"/>
   </sortState>
@@ -1103,8 +1114,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:S21" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:S21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:S23" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:S23"/>
   <sortState ref="A2:BF219">
     <sortCondition ref="A4:A5"/>
   </sortState>
@@ -1399,10 +1410,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1420,24 +1431,23 @@
     <col min="11" max="11" width="5.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.21875" customWidth="1"/>
+    <col min="16" max="16" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
         <v>61</v>
@@ -1446,10 +1456,10 @@
         <v>62</v>
       </c>
       <c r="E1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" t="s">
         <v>101</v>
-      </c>
-      <c r="F1" t="s">
-        <v>102</v>
       </c>
       <c r="G1" t="s">
         <v>63</v>
@@ -1473,34 +1483,31 @@
         <v>69</v>
       </c>
       <c r="N1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="Q1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="R1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="T1" t="s">
+        <v>87</v>
+      </c>
+      <c r="U1" t="s">
         <v>81</v>
       </c>
-      <c r="U1" t="s">
-        <v>88</v>
-      </c>
-      <c r="V1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1508,7 +1515,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D2">
         <v>375</v>
@@ -1535,170 +1542,38 @@
         <v>6.2</v>
       </c>
       <c r="M2">
-        <v>2.44</v>
-      </c>
-      <c r="N2">
-        <v>0.87</v>
+        <v>3.84</v>
+      </c>
+      <c r="N2" t="s">
+        <v>123</v>
       </c>
       <c r="O2" t="s">
-        <v>121</v>
-      </c>
-      <c r="P2" t="s">
-        <v>123</v>
+        <v>124</v>
+      </c>
+      <c r="P2">
+        <v>1.17</v>
       </c>
       <c r="Q2">
-        <v>1.17</v>
+        <v>1.91</v>
       </c>
       <c r="R2">
-        <v>1.91</v>
+        <v>1E-3</v>
       </c>
       <c r="S2">
-        <v>1E-3</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2" t="b">
-        <v>1</v>
-      </c>
-      <c r="V2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3">
-        <v>375</v>
-      </c>
-      <c r="F3">
-        <v>620</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>6.2</v>
-      </c>
-      <c r="M3">
-        <v>2.44</v>
-      </c>
-      <c r="N3">
-        <v>0.87</v>
-      </c>
-      <c r="O3" t="s">
-        <v>121</v>
-      </c>
-      <c r="P3" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q3">
-        <v>1.17</v>
-      </c>
-      <c r="R3">
-        <v>1.91</v>
-      </c>
-      <c r="S3">
-        <v>1E-3</v>
-      </c>
-      <c r="T3">
-        <v>2</v>
-      </c>
-      <c r="U3" t="b">
-        <v>1</v>
-      </c>
-      <c r="V3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4">
-        <v>375</v>
-      </c>
-      <c r="F4">
-        <v>620</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>6.2</v>
-      </c>
-      <c r="M4">
-        <v>2.44</v>
-      </c>
-      <c r="N4">
-        <v>0.87</v>
-      </c>
-      <c r="O4" t="s">
-        <v>121</v>
-      </c>
-      <c r="P4" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q4">
-        <v>1.17</v>
-      </c>
-      <c r="R4">
-        <v>1.91</v>
-      </c>
-      <c r="S4">
-        <v>1E-3</v>
-      </c>
-      <c r="T4">
-        <v>3</v>
-      </c>
-      <c r="U4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V4" t="s">
-        <v>83</v>
+        <v>-1</v>
+      </c>
+      <c r="T2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1708,10 +1583,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B21"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1727,19 +1602,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
         <v>56</v>
       </c>
       <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>86</v>
-      </c>
-      <c r="E1" t="s">
-        <v>87</v>
       </c>
       <c r="F1" t="s">
         <v>70</v>
@@ -2127,46 +2002,67 @@
       <c r="A20" s="28">
         <v>1</v>
       </c>
-      <c r="B20" s="28">
-        <v>263</v>
+      <c r="B20" s="36">
+        <v>845</v>
       </c>
       <c r="C20" s="28">
         <v>0</v>
       </c>
       <c r="D20" s="28">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E20" s="29">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="F20" s="30" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
-        <v>Corn Silage Processed 25 DM 41 NDF Medium</v>
+        <v>UREA</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="28">
+      <c r="A21" s="14">
         <v>1</v>
       </c>
-      <c r="B21" s="36">
-        <v>845</v>
-      </c>
-      <c r="C21" s="28">
-        <v>0</v>
-      </c>
-      <c r="D21" s="28">
+      <c r="B21" s="20">
+        <v>101</v>
+      </c>
+      <c r="C21" s="14">
+        <v>0</v>
+      </c>
+      <c r="D21" s="14">
         <v>100</v>
       </c>
       <c r="E21" s="29">
-        <v>0.4</v>
-      </c>
-      <c r="F21" s="30" t="str">
+        <v>0.3</v>
+      </c>
+      <c r="F21" s="22" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
-        <v>UREA</v>
+        <v>Baled grass, temporary meadow, with clover, Northwestern region, at farm/FR S</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="14">
+        <v>1</v>
+      </c>
+      <c r="B22" s="20">
+        <v>102</v>
+      </c>
+      <c r="C22" s="14">
+        <v>0</v>
+      </c>
+      <c r="D22" s="14">
+        <v>100</v>
+      </c>
+      <c r="E22" s="29">
+        <v>0.3</v>
+      </c>
+      <c r="F22" s="22" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</f>
+        <v>Grass silage, horizontal silo, temporary meadow, with clover, Northwestern region, at farm/FR S</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B21">
+  <conditionalFormatting sqref="B2:B22">
     <cfRule type="expression" dxfId="53" priority="3" stopIfTrue="1">
       <formula>ROW(B2)=$C$1</formula>
     </cfRule>
@@ -2174,17 +2070,18 @@
       <formula>COLUMN(B2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
+  <conditionalFormatting sqref="B20">
     <cfRule type="expression" dxfId="51" priority="1" stopIfTrue="1">
-      <formula>ROW(B21)=$E$1</formula>
+      <formula>ROW(B20)=$E$1</formula>
     </cfRule>
     <cfRule type="expression" dxfId="50" priority="2" stopIfTrue="1">
-      <formula>COLUMN(B21)=$F$1</formula>
+      <formula>COLUMN(B20)=$F$1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2194,10 +2091,10 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2215,34 +2112,34 @@
         <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="16" t="s">
-        <v>100</v>
-      </c>
       <c r="I1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -2271,7 +2168,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K2" t="b">
         <v>0</v>
@@ -2309,7 +2206,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K3" t="b">
         <v>1</v>
@@ -2347,10 +2244,42 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K4" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>0.2</v>
+      </c>
+      <c r="D5">
+        <v>0.2</v>
+      </c>
+      <c r="E5">
+        <v>0.4</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0.2</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2367,10 +2296,10 @@
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A2:A21"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.6640625" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2388,22 +2317,22 @@
         <v>70</v>
       </c>
       <c r="C1" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="19" t="s">
         <v>92</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2944,6 +2873,58 @@
       </c>
       <c r="H21" s="27">
         <v>0.29275619000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="39">
+        <v>101</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="40">
+        <v>7.2338821999999997E-3</v>
+      </c>
+      <c r="D22" s="39">
+        <v>2.1388340000000001</v>
+      </c>
+      <c r="E22" s="39">
+        <v>0.31076082999999999</v>
+      </c>
+      <c r="F22" s="39">
+        <v>3.6478406000000001E-3</v>
+      </c>
+      <c r="G22" s="39">
+        <v>9.9511690999999993E-4</v>
+      </c>
+      <c r="H22" s="39">
+        <v>1.448909</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="39">
+        <v>102</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="40">
+        <v>1.398646E-5</v>
+      </c>
+      <c r="D23" s="39">
+        <v>1.0869945000000001</v>
+      </c>
+      <c r="E23" s="39">
+        <v>0.18026732000000001</v>
+      </c>
+      <c r="F23" s="39">
+        <v>7.1452427000000002E-3</v>
+      </c>
+      <c r="G23" s="39">
+        <v>1.8322938999999999E-3</v>
+      </c>
+      <c r="H23" s="39">
+        <v>1.1594272000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2984,10 +2965,10 @@
   <sheetPr codeName="Sheet5">
     <tabColor theme="2"/>
   </sheetPr>
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A2:A21"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3076,7 +3057,7 @@
         <v>159</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -3135,7 +3116,7 @@
         <v>169</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="3">
         <v>0</v>
@@ -3194,7 +3175,7 @@
         <v>520</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="3">
         <v>0</v>
@@ -3253,7 +3234,7 @@
         <v>242</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
@@ -3312,7 +3293,7 @@
         <v>211</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -3371,7 +3352,7 @@
         <v>511</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
@@ -3430,7 +3411,7 @@
         <v>119</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
@@ -3489,7 +3470,7 @@
         <v>535</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
@@ -3548,7 +3529,7 @@
         <v>539</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -3607,7 +3588,7 @@
         <v>519</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
@@ -3666,7 +3647,7 @@
         <v>525</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" s="3">
         <v>0</v>
@@ -3784,7 +3765,7 @@
         <v>127</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
@@ -3902,7 +3883,7 @@
         <v>508</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -3961,7 +3942,7 @@
         <v>244</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
@@ -4020,7 +4001,7 @@
         <v>248</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
@@ -4138,7 +4119,7 @@
         <v>263</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C20" s="3">
         <v>100</v>
@@ -4197,7 +4178,7 @@
         <v>845</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
@@ -4249,6 +4230,124 @@
       </c>
       <c r="S21" s="3">
         <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="24">
+        <v>101</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="3">
+        <v>100</v>
+      </c>
+      <c r="D22" s="38">
+        <v>70.83</v>
+      </c>
+      <c r="E22" s="38">
+        <v>10.63</v>
+      </c>
+      <c r="F22" s="23">
+        <v>39</v>
+      </c>
+      <c r="G22" s="23">
+        <v>14.3</v>
+      </c>
+      <c r="H22" s="23">
+        <v>0</v>
+      </c>
+      <c r="I22" s="23">
+        <v>0</v>
+      </c>
+      <c r="J22" s="23">
+        <v>2.8</v>
+      </c>
+      <c r="K22" s="38">
+        <v>8.48</v>
+      </c>
+      <c r="L22" s="23">
+        <v>9.89</v>
+      </c>
+      <c r="M22" s="38">
+        <v>46</v>
+      </c>
+      <c r="N22" s="38">
+        <v>2.57</v>
+      </c>
+      <c r="O22" s="3">
+        <v>49.599998474121094</v>
+      </c>
+      <c r="P22" s="3">
+        <v>0.94999998807907104</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>0.40000000596046448</v>
+      </c>
+      <c r="R22" s="23">
+        <v>29</v>
+      </c>
+      <c r="S22" s="23">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="24">
+        <v>102</v>
+      </c>
+      <c r="B23" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="3">
+        <v>100</v>
+      </c>
+      <c r="D23" s="3">
+        <v>33.76</v>
+      </c>
+      <c r="E23" s="3">
+        <v>13.23</v>
+      </c>
+      <c r="F23" s="3">
+        <v>70</v>
+      </c>
+      <c r="G23" s="3">
+        <v>5</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1.62</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
+        <v>2.44</v>
+      </c>
+      <c r="K23" s="3">
+        <v>4.1999998092651367</v>
+      </c>
+      <c r="L23" s="3">
+        <v>32.549999237060547</v>
+      </c>
+      <c r="M23" s="3">
+        <v>53.38</v>
+      </c>
+      <c r="N23" s="3">
+        <v>7</v>
+      </c>
+      <c r="O23" s="3">
+        <v>72.900001525878906</v>
+      </c>
+      <c r="P23" s="3">
+        <v>1.7200000286102295</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>1.1000000238418579</v>
+      </c>
+      <c r="R23" s="3">
+        <v>17</v>
+      </c>
+      <c r="S23" s="3">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4594,6 +4693,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003C4402FDC8975A4FB65AB474AF423692" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="293b87d96ae3165967deaddc9dd3a283">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="871f9270-bc3b-4105-9923-e7982e1cb312" xmlns:ns4="000447b7-86fa-4362-939e-855579e16124" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="23a07973a4b986d214a26a52ed717842" ns3:_="" ns4:_="">
     <xsd:import namespace="871f9270-bc3b-4105-9923-e7982e1cb312"/>
@@ -4810,36 +4924,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C172DDCE-6A5B-4F5B-846C-532884D79266}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
-    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4862,9 +4950,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C172DDCE-6A5B-4F5B-846C-532884D79266}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
+    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DMIeq 1996 and 2016 implemented. DMI calculation fixed
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="134">
   <si>
     <t>IFN</t>
   </si>
@@ -404,6 +404,33 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>GSS-MAX_CO2</t>
+  </si>
+  <si>
+    <t>GSS-MAX_BALANCED_N</t>
+  </si>
+  <si>
+    <t>GSS-MAX_BALANCED_FLOR</t>
+  </si>
+  <si>
+    <t>GSS</t>
+  </si>
+  <si>
+    <t>GSS-MAX_BALANCED</t>
+  </si>
+  <si>
+    <t>GSS-MAX_BALANCED_FLOR_N</t>
+  </si>
+  <si>
+    <t>GSS-MAX_CO2_MONO</t>
+  </si>
+  <si>
+    <t>DMI Equation</t>
+  </si>
+  <si>
+    <t>NRC2016</t>
   </si>
 </sst>
 </file>
@@ -603,6 +630,134 @@
   </cellStyles>
   <dxfs count="54">
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
@@ -713,54 +868,6 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -868,54 +975,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -976,38 +1035,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1022,9 +1049,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:U2" totalsRowShown="0">
-  <autoFilter ref="A1:U2"/>
-  <tableColumns count="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:V8" totalsRowShown="0">
+  <autoFilter ref="A1:V8"/>
+  <tableColumns count="22">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Feed Scenario"/>
     <tableColumn id="3" name="Breed"/>
@@ -1043,6 +1070,7 @@
     <tableColumn id="17" name="LB"/>
     <tableColumn id="18" name="UB"/>
     <tableColumn id="19" name="Tol"/>
+    <tableColumn id="14" name="DMI Equation"/>
     <tableColumn id="20" name="LCA ID"/>
     <tableColumn id="21" name="Multiobjective"/>
     <tableColumn id="22" name="Obj"/>
@@ -1052,18 +1080,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F22" totalsRowShown="0" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F22" totalsRowShown="0" dataDxfId="53">
   <autoFilter ref="A1:F22"/>
   <sortState ref="B2:F30">
     <sortCondition ref="B1:B30"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="6" name="Feed Scenario" dataDxfId="48"/>
-    <tableColumn id="1" name="ID" dataDxfId="47"/>
-    <tableColumn id="2" name="Min %DM" dataDxfId="46"/>
-    <tableColumn id="3" name="Max %DM" dataDxfId="45"/>
-    <tableColumn id="4" name="Cost [US$/kg AF]" dataDxfId="44"/>
-    <tableColumn id="5" name="Name" dataDxfId="43">
+    <tableColumn id="6" name="Feed Scenario" dataDxfId="52"/>
+    <tableColumn id="1" name="ID" dataDxfId="51"/>
+    <tableColumn id="2" name="Min %DM" dataDxfId="50"/>
+    <tableColumn id="3" name="Max %DM" dataDxfId="49"/>
+    <tableColumn id="4" name="Cost [US$/kg AF]" dataDxfId="48"/>
+    <tableColumn id="5" name="Name" dataDxfId="47">
       <calculatedColumnFormula>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[#Data],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1072,8 +1100,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:K5" totalsRowShown="0">
-  <autoFilter ref="A1:K5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:K6" totalsRowShown="0">
+  <autoFilter ref="A1:K6"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="4" name="LCA weight"/>
@@ -1092,53 +1120,53 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela26" displayName="Tabela26" ref="A1:H23" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela26" displayName="Tabela26" ref="A1:H23" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:H23"/>
   <sortState ref="A2:C15">
     <sortCondition ref="A1:A15"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="ID" dataDxfId="34"/>
-    <tableColumn id="5" name="Name" dataDxfId="33">
+    <tableColumn id="1" name="ID" dataDxfId="44"/>
+    <tableColumn id="5" name="Name" dataDxfId="43">
       <calculatedColumnFormula>VLOOKUP(Tabela26[[#This Row],[ID]],FeedLib[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="LCA_Phosphorous consumption (kg P)" dataDxfId="32"/>
-    <tableColumn id="3" name="LCA_CED 1.8 non renewable fossil+nuclear (MJ)" dataDxfId="31"/>
-    <tableColumn id="4" name="LCA_Climate change ILCD (kg CO2 eq)" dataDxfId="30"/>
-    <tableColumn id="7" name="LCA_Acidification ILCD (molc H+ eq)" dataDxfId="29"/>
-    <tableColumn id="8" name="LCA_Eutrophication CML baseline (kg PO4- eq)" dataDxfId="28"/>
-    <tableColumn id="9" name="LCA_Land competition CML non baseline (m2a)" dataDxfId="27"/>
+    <tableColumn id="2" name="LCA_Phosphorous consumption (kg P)" dataDxfId="42"/>
+    <tableColumn id="3" name="LCA_CED 1.8 non renewable fossil+nuclear (MJ)" dataDxfId="41"/>
+    <tableColumn id="4" name="LCA_Climate change ILCD (kg CO2 eq)" dataDxfId="40"/>
+    <tableColumn id="7" name="LCA_Acidification ILCD (molc H+ eq)" dataDxfId="39"/>
+    <tableColumn id="8" name="LCA_Eutrophication CML baseline (kg PO4- eq)" dataDxfId="38"/>
+    <tableColumn id="9" name="LCA_Land competition CML non baseline (m2a)" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:S23" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:S23" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A1:S23"/>
   <sortState ref="A2:BF219">
     <sortCondition ref="A4:A5"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" name="ID" dataDxfId="18"/>
-    <tableColumn id="2" name="Feed" dataDxfId="17"/>
-    <tableColumn id="7" name="Forage, %DM" dataDxfId="16"/>
-    <tableColumn id="8" name="DM, %AF" dataDxfId="15"/>
-    <tableColumn id="16" name="CP, %DM" dataDxfId="14"/>
-    <tableColumn id="31" name="SP, %CP" dataDxfId="13"/>
-    <tableColumn id="29" name="ADICP, %CP" dataDxfId="12"/>
-    <tableColumn id="24" name="Sugars, %DM" dataDxfId="11"/>
-    <tableColumn id="25" name="OA, %DM" dataDxfId="10"/>
-    <tableColumn id="23" name="Fat, %DM" dataDxfId="9"/>
-    <tableColumn id="9" name="Ash, %DM" dataDxfId="8"/>
-    <tableColumn id="10" name="Starch, %DM" dataDxfId="7"/>
-    <tableColumn id="12" name="NDF, %DM" dataDxfId="6"/>
-    <tableColumn id="13" name="Lignin, %DM" dataDxfId="5"/>
-    <tableColumn id="14" name="TDN, %DM" dataDxfId="4"/>
-    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="3"/>
-    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="2"/>
-    <tableColumn id="21" name="RUP, %CP" dataDxfId="1"/>
-    <tableColumn id="20" name="pef, %NDF" dataDxfId="0"/>
+    <tableColumn id="1" name="ID" dataDxfId="34"/>
+    <tableColumn id="2" name="Feed" dataDxfId="33"/>
+    <tableColumn id="7" name="Forage, %DM" dataDxfId="32"/>
+    <tableColumn id="8" name="DM, %AF" dataDxfId="31"/>
+    <tableColumn id="16" name="CP, %DM" dataDxfId="30"/>
+    <tableColumn id="31" name="SP, %CP" dataDxfId="29"/>
+    <tableColumn id="29" name="ADICP, %CP" dataDxfId="28"/>
+    <tableColumn id="24" name="Sugars, %DM" dataDxfId="27"/>
+    <tableColumn id="25" name="OA, %DM" dataDxfId="26"/>
+    <tableColumn id="23" name="Fat, %DM" dataDxfId="25"/>
+    <tableColumn id="9" name="Ash, %DM" dataDxfId="24"/>
+    <tableColumn id="10" name="Starch, %DM" dataDxfId="23"/>
+    <tableColumn id="12" name="NDF, %DM" dataDxfId="22"/>
+    <tableColumn id="13" name="Lignin, %DM" dataDxfId="21"/>
+    <tableColumn id="14" name="TDN, %DM" dataDxfId="20"/>
+    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="19"/>
+    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="18"/>
+    <tableColumn id="21" name="RUP, %CP" dataDxfId="17"/>
+    <tableColumn id="20" name="pef, %NDF" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1410,10 +1438,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="S2" sqref="S2:S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1432,17 +1460,18 @@
     <col min="12" max="12" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.21875" customWidth="1"/>
+    <col min="15" max="15" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5.21875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.88671875" customWidth="1"/>
+    <col min="19" max="19" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -1498,16 +1527,19 @@
         <v>75</v>
       </c>
       <c r="S1" t="s">
+        <v>132</v>
+      </c>
+      <c r="T1" t="s">
         <v>80</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>87</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1551,21 +1583,414 @@
         <v>124</v>
       </c>
       <c r="P2">
-        <v>1.17</v>
+        <v>0.96</v>
       </c>
       <c r="Q2">
-        <v>1.91</v>
+        <v>2.02</v>
       </c>
       <c r="R2">
         <v>1E-3</v>
       </c>
-      <c r="S2">
+      <c r="S2" t="s">
+        <v>133</v>
+      </c>
+      <c r="T2">
         <v>-1</v>
       </c>
-      <c r="T2" t="b">
-        <v>0</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="U2" t="b">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3">
+        <v>375</v>
+      </c>
+      <c r="F3">
+        <v>620</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>6.2</v>
+      </c>
+      <c r="M3">
+        <v>3.84</v>
+      </c>
+      <c r="N3" t="s">
+        <v>128</v>
+      </c>
+      <c r="O3" t="s">
+        <v>131</v>
+      </c>
+      <c r="P3">
+        <v>0.96</v>
+      </c>
+      <c r="Q3">
+        <v>2.02</v>
+      </c>
+      <c r="R3">
+        <v>1E-3</v>
+      </c>
+      <c r="S3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3" t="b">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4">
+        <v>375</v>
+      </c>
+      <c r="F4">
+        <v>620</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>6.2</v>
+      </c>
+      <c r="M4">
+        <v>3.84</v>
+      </c>
+      <c r="N4" t="s">
+        <v>128</v>
+      </c>
+      <c r="O4" t="s">
+        <v>125</v>
+      </c>
+      <c r="P4">
+        <v>0.96</v>
+      </c>
+      <c r="Q4">
+        <v>2.02</v>
+      </c>
+      <c r="R4">
+        <v>1E-3</v>
+      </c>
+      <c r="S4" t="s">
+        <v>133</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" t="b">
+        <v>1</v>
+      </c>
+      <c r="V4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5">
+        <v>375</v>
+      </c>
+      <c r="F5">
+        <v>620</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>6.2</v>
+      </c>
+      <c r="M5">
+        <v>3.84</v>
+      </c>
+      <c r="N5" t="s">
+        <v>128</v>
+      </c>
+      <c r="O5" t="s">
+        <v>126</v>
+      </c>
+      <c r="P5">
+        <v>0.96</v>
+      </c>
+      <c r="Q5">
+        <v>2.02</v>
+      </c>
+      <c r="R5">
+        <v>1E-3</v>
+      </c>
+      <c r="S5" t="s">
+        <v>133</v>
+      </c>
+      <c r="T5">
+        <v>2</v>
+      </c>
+      <c r="U5" t="b">
+        <v>1</v>
+      </c>
+      <c r="V5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6">
+        <v>375</v>
+      </c>
+      <c r="F6">
+        <v>620</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>6.2</v>
+      </c>
+      <c r="M6">
+        <v>3.84</v>
+      </c>
+      <c r="N6" t="s">
+        <v>128</v>
+      </c>
+      <c r="O6" t="s">
+        <v>129</v>
+      </c>
+      <c r="P6">
+        <v>0.96</v>
+      </c>
+      <c r="Q6">
+        <v>2.02</v>
+      </c>
+      <c r="R6">
+        <v>1E-3</v>
+      </c>
+      <c r="S6" t="s">
+        <v>133</v>
+      </c>
+      <c r="T6">
+        <v>3</v>
+      </c>
+      <c r="U6" t="b">
+        <v>1</v>
+      </c>
+      <c r="V6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7">
+        <v>375</v>
+      </c>
+      <c r="F7">
+        <v>620</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>6.2</v>
+      </c>
+      <c r="M7">
+        <v>3.84</v>
+      </c>
+      <c r="N7" t="s">
+        <v>128</v>
+      </c>
+      <c r="O7" t="s">
+        <v>130</v>
+      </c>
+      <c r="P7">
+        <v>0.96</v>
+      </c>
+      <c r="Q7">
+        <v>2.02</v>
+      </c>
+      <c r="R7">
+        <v>1E-3</v>
+      </c>
+      <c r="S7" t="s">
+        <v>133</v>
+      </c>
+      <c r="T7">
+        <v>4</v>
+      </c>
+      <c r="U7" t="b">
+        <v>1</v>
+      </c>
+      <c r="V7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8">
+        <v>375</v>
+      </c>
+      <c r="F8">
+        <v>620</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>6.2</v>
+      </c>
+      <c r="M8">
+        <v>3.84</v>
+      </c>
+      <c r="N8" t="s">
+        <v>128</v>
+      </c>
+      <c r="O8" t="s">
+        <v>127</v>
+      </c>
+      <c r="P8">
+        <v>0.96</v>
+      </c>
+      <c r="Q8">
+        <v>2.02</v>
+      </c>
+      <c r="R8">
+        <v>1E-3</v>
+      </c>
+      <c r="S8" t="s">
+        <v>133</v>
+      </c>
+      <c r="T8">
+        <v>5</v>
+      </c>
+      <c r="U8" t="b">
+        <v>1</v>
+      </c>
+      <c r="V8" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2063,18 +2488,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B22">
-    <cfRule type="expression" dxfId="53" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
       <formula>ROW(B2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
       <formula>COLUMN(B2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="expression" dxfId="51" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
       <formula>ROW(B20)=$E$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="2" stopIfTrue="1">
       <formula>COLUMN(B20)=$F$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2091,10 +2516,10 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2280,6 +2705,38 @@
       </c>
       <c r="K5" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0.2</v>
+      </c>
+      <c r="D6">
+        <v>0.2</v>
+      </c>
+      <c r="E6">
+        <v>0.4</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0.2</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2929,26 +3386,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A19">
-    <cfRule type="expression" dxfId="42" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
       <formula>ROW(A2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
       <formula>COLUMN(A2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="40" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
       <formula>ROW(A21)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
       <formula>COLUMN(A21)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="38" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
       <formula>ROW(A21)=$E$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>COLUMN(A21)=$F$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4352,26 +4809,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S20 A21:B21 S21">
-    <cfRule type="expression" dxfId="26" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>ROW(A2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
       <formula>COLUMN(A2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="expression" dxfId="24" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>ROW(C21)=$E$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>COLUMN(C21)=$F$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N21:R21">
-    <cfRule type="expression" dxfId="22" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>ROW(N21)=$E$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>COLUMN(N21)=$F$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4693,21 +5150,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003C4402FDC8975A4FB65AB474AF423692" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="293b87d96ae3165967deaddc9dd3a283">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="871f9270-bc3b-4105-9923-e7982e1cb312" xmlns:ns4="000447b7-86fa-4362-939e-855579e16124" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="23a07973a4b986d214a26a52ed717842" ns3:_="" ns4:_="">
     <xsd:import namespace="871f9270-bc3b-4105-9923-e7982e1cb312"/>
@@ -4924,32 +5366,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C172DDCE-6A5B-4F5B-846C-532884D79266}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4966,4 +5398,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DMI calculation fixed: not imported from RData anymore, instead averaged
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -497,7 +497,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="162">
   <si>
     <t>Feed Scenario</t>
   </si>
@@ -829,16 +829,7 @@
     <t>LCA_Land competition CML non baseline (m2a)</t>
   </si>
   <si>
-    <t>GSS-MAX_BIS_N</t>
-  </si>
-  <si>
     <t>GSS-MAX_BIS_F_N</t>
-  </si>
-  <si>
-    <t>GSS-MAX_BIS_F</t>
-  </si>
-  <si>
-    <t>GSS-MAX_BIS</t>
   </si>
   <si>
     <t>NPN, %DM</t>
@@ -1002,7 +993,7 @@
     <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1151,17 +1142,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF080808"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1226,7 +1206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1263,30 +1243,6 @@
         <color rgb="FF5B9BD5"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1345,7 +1301,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1370,20 +1326,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1394,14 +1347,14 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1429,11 +1382,11 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1446,20 +1399,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2729,6 +2685,7 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -6742,7 +6699,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6796,7 +6753,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6850,7 +6807,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7401,8 +7358,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="scenario" displayName="scenario" ref="A1:X8" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66" tableBorderDxfId="65">
-  <autoFilter ref="A1:X8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="scenario" displayName="scenario" ref="A1:X5" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66" tableBorderDxfId="65">
+  <autoFilter ref="A1:X5"/>
   <tableColumns count="24">
     <tableColumn id="1" name="ID" dataDxfId="64"/>
     <tableColumn id="2" name="Feed Scenario" dataDxfId="63"/>
@@ -7519,7 +7476,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela26" displayName="Tabela26" ref="A1:H22" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:H22"/>
   <sortState ref="A2:H22">
-    <sortCondition ref="A1:A22"/>
+    <sortCondition ref="E1:E22"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" name="ID" dataDxfId="7" dataCellStyle="Normal 3"/>
@@ -7804,7 +7761,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7842,16 +7799,16 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="28">
         <v>3</v>
       </c>
-      <c r="C2" s="30">
-        <v>0</v>
-      </c>
-      <c r="D2" s="30">
+      <c r="C2" s="27">
+        <v>0</v>
+      </c>
+      <c r="D2" s="27">
         <v>4</v>
       </c>
-      <c r="E2" s="45">
+      <c r="E2" s="42">
         <v>0.39074999999999999</v>
       </c>
       <c r="F2" s="16" t="str">
@@ -7863,16 +7820,16 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="28">
         <v>4</v>
       </c>
       <c r="C3" s="17">
         <v>0</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="27">
         <v>40</v>
       </c>
-      <c r="E3" s="44">
+      <c r="E3" s="41">
         <v>0.22500000000000001</v>
       </c>
       <c r="F3" s="16" t="str">
@@ -7884,7 +7841,7 @@
       <c r="A4" s="16">
         <v>1</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="28">
         <v>5</v>
       </c>
       <c r="C4" s="17">
@@ -7893,7 +7850,7 @@
       <c r="D4" s="17">
         <v>30</v>
       </c>
-      <c r="E4" s="44">
+      <c r="E4" s="41">
         <v>0.22575000000000001</v>
       </c>
       <c r="F4" s="16" t="str">
@@ -7905,7 +7862,7 @@
       <c r="A5" s="16">
         <v>1</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="28">
         <v>6</v>
       </c>
       <c r="C5" s="17">
@@ -7914,7 +7871,7 @@
       <c r="D5" s="17">
         <v>20</v>
       </c>
-      <c r="E5" s="44">
+      <c r="E5" s="41">
         <v>0.78425</v>
       </c>
       <c r="F5" s="16" t="str">
@@ -7926,7 +7883,7 @@
       <c r="A6" s="16">
         <v>1</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="28">
         <v>8</v>
       </c>
       <c r="C6" s="17">
@@ -7935,7 +7892,7 @@
       <c r="D6" s="17">
         <v>8</v>
       </c>
-      <c r="E6" s="44">
+      <c r="E6" s="41">
         <v>0.23025000000000001</v>
       </c>
       <c r="F6" s="16" t="str">
@@ -7947,7 +7904,7 @@
       <c r="A7" s="16">
         <v>1</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="28">
         <v>9</v>
       </c>
       <c r="C7" s="17">
@@ -7956,7 +7913,7 @@
       <c r="D7" s="17">
         <v>50</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="41">
         <v>0.26624999999999999</v>
       </c>
       <c r="F7" s="16" t="str">
@@ -7968,16 +7925,16 @@
       <c r="A8" s="16">
         <v>1</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="28">
         <v>10</v>
       </c>
       <c r="C8" s="17">
         <v>0</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="27">
         <v>2</v>
       </c>
-      <c r="E8" s="44">
+      <c r="E8" s="41">
         <v>0.91974999999999996</v>
       </c>
       <c r="F8" s="16" t="str">
@@ -7989,16 +7946,16 @@
       <c r="A9" s="16">
         <v>1</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="28">
         <v>12</v>
       </c>
       <c r="C9" s="17">
         <v>0</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="27">
         <v>30</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="41">
         <v>0.182</v>
       </c>
       <c r="F9" s="16" t="str">
@@ -8010,16 +7967,16 @@
       <c r="A10" s="16">
         <v>1</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="28">
         <v>16</v>
       </c>
       <c r="C10" s="17">
         <v>0</v>
       </c>
-      <c r="D10" s="30">
-        <v>2</v>
-      </c>
-      <c r="E10" s="44">
+      <c r="D10" s="27">
+        <v>0</v>
+      </c>
+      <c r="E10" s="41">
         <v>0.89075000000000004</v>
       </c>
       <c r="F10" s="16" t="str">
@@ -8031,16 +7988,16 @@
       <c r="A11" s="16">
         <v>1</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="28">
         <v>17</v>
       </c>
       <c r="C11" s="17">
         <v>0</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="27">
         <v>30</v>
       </c>
-      <c r="E11" s="44">
+      <c r="E11" s="41">
         <v>0.1305</v>
       </c>
       <c r="F11" s="16" t="str">
@@ -8052,16 +8009,16 @@
       <c r="A12" s="16">
         <v>1</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="28">
         <v>18</v>
       </c>
       <c r="C12" s="17">
         <v>0</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="27">
         <v>30</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="41">
         <v>0.3095</v>
       </c>
       <c r="F12" s="16" t="str">
@@ -8073,16 +8030,16 @@
       <c r="A13" s="16">
         <v>1</v>
       </c>
-      <c r="B13" s="31">
+      <c r="B13" s="28">
         <v>19</v>
       </c>
       <c r="C13" s="17">
         <v>0</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="27">
         <v>30</v>
       </c>
-      <c r="E13" s="44">
+      <c r="E13" s="41">
         <v>0.222</v>
       </c>
       <c r="F13" s="16" t="str">
@@ -8094,19 +8051,19 @@
       <c r="A14" s="16">
         <v>1</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="28">
         <v>20</v>
       </c>
       <c r="C14" s="17">
         <v>0</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="27">
         <v>40</v>
       </c>
-      <c r="E14" s="44">
+      <c r="E14" s="41">
         <v>0.20399999999999999</v>
       </c>
-      <c r="F14" s="53" t="str">
+      <c r="F14" s="50" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[#Data],2,0)</f>
         <v>Wheat gluten feed</v>
       </c>
@@ -8115,16 +8072,16 @@
       <c r="A15" s="16">
         <v>1</v>
       </c>
-      <c r="B15" s="31">
+      <c r="B15" s="28">
         <v>21</v>
       </c>
       <c r="C15" s="17">
         <v>0</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="27">
         <v>30</v>
       </c>
-      <c r="E15" s="44">
+      <c r="E15" s="41">
         <v>0.16425000000000001</v>
       </c>
       <c r="F15" s="16" t="str">
@@ -8136,16 +8093,16 @@
       <c r="A16" s="16">
         <v>1</v>
       </c>
-      <c r="B16" s="31">
+      <c r="B16" s="28">
         <v>25</v>
       </c>
       <c r="C16" s="17">
         <v>0</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="27">
         <v>100</v>
       </c>
-      <c r="E16" s="44">
+      <c r="E16" s="41">
         <v>9.0749999999999997E-2</v>
       </c>
       <c r="F16" s="16" t="str">
@@ -8157,16 +8114,16 @@
       <c r="A17" s="16">
         <v>1</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="28">
         <v>28</v>
       </c>
       <c r="C17" s="17">
         <v>0</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="27">
         <v>10</v>
       </c>
-      <c r="E17" s="44">
+      <c r="E17" s="41">
         <v>0.24766666666666665</v>
       </c>
       <c r="F17" s="16" t="str">
@@ -8178,16 +8135,16 @@
       <c r="A18" s="16">
         <v>1</v>
       </c>
-      <c r="B18" s="31">
+      <c r="B18" s="28">
         <v>29</v>
       </c>
       <c r="C18" s="17">
         <v>0</v>
       </c>
-      <c r="D18" s="49">
+      <c r="D18" s="46">
         <v>10</v>
       </c>
-      <c r="E18" s="54">
+      <c r="E18" s="51">
         <v>0.29599999999999999</v>
       </c>
       <c r="F18" s="16" t="str">
@@ -8199,7 +8156,7 @@
       <c r="A19" s="16">
         <v>1</v>
       </c>
-      <c r="B19" s="31">
+      <c r="B19" s="28">
         <v>30</v>
       </c>
       <c r="C19" s="17">
@@ -8208,7 +8165,7 @@
       <c r="D19" s="17">
         <v>100</v>
       </c>
-      <c r="E19" s="45">
+      <c r="E19" s="42">
         <v>5.2600000000000001E-2</v>
       </c>
       <c r="F19" s="16" t="str">
@@ -8220,7 +8177,7 @@
       <c r="A20" s="16">
         <v>1</v>
       </c>
-      <c r="B20" s="31">
+      <c r="B20" s="28">
         <v>31</v>
       </c>
       <c r="C20" s="17">
@@ -8229,7 +8186,7 @@
       <c r="D20" s="17">
         <v>100</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="42">
         <v>7.6749999999999999E-2</v>
       </c>
       <c r="F20" s="16" t="str">
@@ -8252,111 +8209,103 @@
   <sheetPr codeName="Planilha2">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:X40"/>
+  <dimension ref="A1:X69"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="42.28515625" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:24" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="P1" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="R1" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="23" t="s">
+      <c r="S1" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="23" t="s">
+      <c r="T1" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="23" t="s">
+      <c r="U1" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="23" t="s">
+      <c r="V1" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="W1" s="23" t="s">
+      <c r="W1" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="X1" s="66" t="s">
         <v>92</v>
       </c>
     </row>
@@ -8371,7 +8320,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E2" s="19">
         <v>336</v>
@@ -8383,7 +8332,7 @@
         <v>595</v>
       </c>
       <c r="H2" s="19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I2" s="19">
         <v>1</v>
@@ -8404,16 +8353,16 @@
         <v>2.41</v>
       </c>
       <c r="O2" s="19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="Q2" s="19">
-        <v>1.3</v>
+        <v>0.7</v>
       </c>
       <c r="R2" s="19">
-        <v>2.1</v>
+        <v>3</v>
       </c>
       <c r="S2" s="19">
         <v>0.01</v>
@@ -8445,7 +8394,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E3" s="19">
         <v>336</v>
@@ -8457,7 +8406,7 @@
         <v>595</v>
       </c>
       <c r="H3" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I3" s="22">
         <v>1</v>
@@ -8481,13 +8430,13 @@
         <v>93</v>
       </c>
       <c r="P3" s="22" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q3" s="19">
-        <v>1.78</v>
+        <v>1.43</v>
       </c>
       <c r="R3" s="19">
-        <v>1.92</v>
+        <v>2.09</v>
       </c>
       <c r="S3" s="22">
         <v>1E-3</v>
@@ -8509,374 +8458,164 @@
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="65">
+      <c r="A4" s="19">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22">
+        <v>1</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="19">
+        <v>336</v>
+      </c>
+      <c r="F4" s="19">
+        <v>0</v>
+      </c>
+      <c r="G4" s="18">
+        <v>595</v>
+      </c>
+      <c r="H4" s="22">
+        <v>6</v>
+      </c>
+      <c r="I4" s="22">
+        <v>1</v>
+      </c>
+      <c r="J4" s="22">
+        <v>1</v>
+      </c>
+      <c r="K4" s="22">
+        <v>1</v>
+      </c>
+      <c r="L4" s="22">
+        <v>0</v>
+      </c>
+      <c r="M4" s="19">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="N4" s="20">
+        <v>2.41</v>
+      </c>
+      <c r="O4" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="P4" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q4" s="19">
+        <v>1.75</v>
+      </c>
+      <c r="R4" s="19">
+        <v>1.9</v>
+      </c>
+      <c r="S4" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="T4" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="U4" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="V4" s="22">
+        <v>0</v>
+      </c>
+      <c r="W4" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="X4" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="59">
         <v>-1</v>
       </c>
-      <c r="B4" s="66">
+      <c r="B5" s="60">
         <v>1</v>
       </c>
-      <c r="C4" s="65">
-        <v>0</v>
-      </c>
-      <c r="D4" s="66" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" s="65">
+      <c r="C5" s="59">
+        <v>0</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="59">
         <v>336</v>
       </c>
-      <c r="F4" s="65">
-        <v>0</v>
-      </c>
-      <c r="G4" s="67">
+      <c r="F5" s="59">
+        <v>0</v>
+      </c>
+      <c r="G5" s="61">
         <v>595</v>
       </c>
-      <c r="H4" s="66">
+      <c r="H5" s="60">
+        <v>6</v>
+      </c>
+      <c r="I5" s="60">
+        <v>1</v>
+      </c>
+      <c r="J5" s="60">
+        <v>1</v>
+      </c>
+      <c r="K5" s="60">
+        <v>1</v>
+      </c>
+      <c r="L5" s="60">
+        <v>0</v>
+      </c>
+      <c r="M5" s="59">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="N5" s="62">
+        <v>2.41</v>
+      </c>
+      <c r="O5" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="P5" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q5" s="19">
+        <v>1.75</v>
+      </c>
+      <c r="R5" s="19">
+        <v>1.9</v>
+      </c>
+      <c r="S5" s="60">
+        <v>1E-3</v>
+      </c>
+      <c r="T5" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="U5" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="V5" s="60">
+        <v>0</v>
+      </c>
+      <c r="W5" s="60">
+        <v>0.1</v>
+      </c>
+      <c r="X5" s="63">
         <v>5</v>
       </c>
-      <c r="I4" s="66">
-        <v>1</v>
-      </c>
-      <c r="J4" s="66">
-        <v>1</v>
-      </c>
-      <c r="K4" s="66">
-        <v>1</v>
-      </c>
-      <c r="L4" s="66">
-        <v>0</v>
-      </c>
-      <c r="M4" s="65">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="N4" s="68">
-        <v>2.41</v>
-      </c>
-      <c r="O4" s="66" t="s">
-        <v>93</v>
-      </c>
-      <c r="P4" s="66" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q4" s="65">
-        <v>1.3</v>
-      </c>
-      <c r="R4" s="65">
-        <v>2.1</v>
-      </c>
-      <c r="S4" s="66">
-        <v>0.01</v>
-      </c>
-      <c r="T4" s="66" t="s">
-        <v>90</v>
-      </c>
-      <c r="U4" s="66" t="s">
-        <v>88</v>
-      </c>
-      <c r="V4" s="66">
-        <v>0</v>
-      </c>
-      <c r="W4" s="66">
-        <v>0.1</v>
-      </c>
-      <c r="X4" s="69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="65">
-        <v>-1</v>
-      </c>
-      <c r="B5" s="65">
-        <v>1</v>
-      </c>
-      <c r="C5" s="65">
-        <v>0</v>
-      </c>
-      <c r="D5" s="65" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="65">
-        <v>336</v>
-      </c>
-      <c r="F5" s="65">
-        <v>0</v>
-      </c>
-      <c r="G5" s="67">
-        <v>595</v>
-      </c>
-      <c r="H5" s="65">
-        <v>5</v>
-      </c>
-      <c r="I5" s="65">
-        <v>1</v>
-      </c>
-      <c r="J5" s="65">
-        <v>1</v>
-      </c>
-      <c r="K5" s="65">
-        <v>1</v>
-      </c>
-      <c r="L5" s="65">
-        <v>0</v>
-      </c>
-      <c r="M5" s="65">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="N5" s="68">
-        <v>2.41</v>
-      </c>
-      <c r="O5" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="P5" s="65" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q5" s="65">
-        <v>1.3</v>
-      </c>
-      <c r="R5" s="65">
-        <v>2.1</v>
-      </c>
-      <c r="S5" s="66">
-        <v>0.01</v>
-      </c>
-      <c r="T5" s="65" t="s">
-        <v>90</v>
-      </c>
-      <c r="U5" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="V5" s="65">
-        <v>0</v>
-      </c>
-      <c r="W5" s="65">
-        <v>0.1</v>
-      </c>
-      <c r="X5" s="67">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
-        <v>5</v>
-      </c>
-      <c r="B6" s="22">
-        <v>1</v>
-      </c>
-      <c r="C6" s="19">
-        <v>0</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="E6" s="19">
-        <v>336</v>
-      </c>
-      <c r="F6" s="19">
-        <v>0</v>
-      </c>
-      <c r="G6" s="18">
-        <v>595</v>
-      </c>
-      <c r="H6" s="22">
-        <v>5</v>
-      </c>
-      <c r="I6" s="22">
-        <v>1</v>
-      </c>
-      <c r="J6" s="22">
-        <v>1</v>
-      </c>
-      <c r="K6" s="22">
-        <v>1</v>
-      </c>
-      <c r="L6" s="22">
-        <v>0</v>
-      </c>
-      <c r="M6" s="19">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="N6" s="20">
-        <v>2.41</v>
-      </c>
-      <c r="O6" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="P6" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q6" s="19">
-        <v>1.78</v>
-      </c>
-      <c r="R6" s="19">
-        <v>1.92</v>
-      </c>
-      <c r="S6" s="22">
-        <v>1E-3</v>
-      </c>
-      <c r="T6" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="U6" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="V6" s="22">
-        <v>0</v>
-      </c>
-      <c r="W6" s="22">
-        <v>0.1</v>
-      </c>
-      <c r="X6" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="65">
-        <v>-1</v>
-      </c>
-      <c r="B7" s="71">
-        <v>1</v>
-      </c>
-      <c r="C7" s="65">
-        <v>0</v>
-      </c>
-      <c r="D7" s="71" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" s="65">
-        <v>336</v>
-      </c>
-      <c r="F7" s="65">
-        <v>0</v>
-      </c>
-      <c r="G7" s="67">
-        <v>595</v>
-      </c>
-      <c r="H7" s="71">
-        <v>5</v>
-      </c>
-      <c r="I7" s="71">
-        <v>1</v>
-      </c>
-      <c r="J7" s="71">
-        <v>1</v>
-      </c>
-      <c r="K7" s="71">
-        <v>1</v>
-      </c>
-      <c r="L7" s="71">
-        <v>0</v>
-      </c>
-      <c r="M7" s="65">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="N7" s="68">
-        <v>2.41</v>
-      </c>
-      <c r="O7" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="P7" s="71" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q7" s="65">
-        <v>1.3</v>
-      </c>
-      <c r="R7" s="65">
-        <v>2.1</v>
-      </c>
-      <c r="S7" s="66">
-        <v>0.01</v>
-      </c>
-      <c r="T7" s="71" t="s">
-        <v>90</v>
-      </c>
-      <c r="U7" s="71" t="s">
-        <v>88</v>
-      </c>
-      <c r="V7" s="71">
-        <v>0</v>
-      </c>
-      <c r="W7" s="71">
-        <v>0.1</v>
-      </c>
-      <c r="X7" s="70">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="62">
-        <v>-1</v>
-      </c>
-      <c r="B8" s="62">
-        <v>1</v>
-      </c>
-      <c r="C8" s="62">
-        <v>0</v>
-      </c>
-      <c r="D8" s="62" t="s">
-        <v>118</v>
-      </c>
-      <c r="E8" s="62">
-        <v>336</v>
-      </c>
-      <c r="F8" s="62">
-        <v>0</v>
-      </c>
-      <c r="G8" s="63">
-        <v>595</v>
-      </c>
-      <c r="H8" s="62">
-        <v>5</v>
-      </c>
-      <c r="I8" s="62">
-        <v>1</v>
-      </c>
-      <c r="J8" s="62">
-        <v>1</v>
-      </c>
-      <c r="K8" s="62">
-        <v>1</v>
-      </c>
-      <c r="L8" s="62">
-        <v>0</v>
-      </c>
-      <c r="M8" s="62">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="N8" s="64">
-        <v>2.41</v>
-      </c>
-      <c r="O8" s="62" t="s">
-        <v>93</v>
-      </c>
-      <c r="P8" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q8" s="62">
-        <v>1.6</v>
-      </c>
-      <c r="R8" s="62">
-        <v>1.61</v>
-      </c>
-      <c r="S8" s="22">
-        <v>1E-3</v>
-      </c>
-      <c r="T8" s="62" t="s">
-        <v>90</v>
-      </c>
-      <c r="U8" s="62" t="s">
-        <v>88</v>
-      </c>
-      <c r="V8" s="62">
-        <v>0</v>
-      </c>
-      <c r="W8" s="62">
-        <v>0.1</v>
-      </c>
-      <c r="X8" s="63">
-        <v>4</v>
-      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F18"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F19"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F20"/>
+      <c r="H20" s="2"/>
     </row>
     <row r="21" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F21"/>
@@ -8887,15 +8626,18 @@
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F23"/>
+      <c r="E23" s="2"/>
+      <c r="G23"/>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F24"/>
+      <c r="E24" s="2"/>
+      <c r="G24"/>
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F25"/>
+      <c r="E25" s="2"/>
+      <c r="G25"/>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="5:8" x14ac:dyDescent="0.25">
@@ -8933,30 +8675,69 @@
       <c r="G32"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E33" s="2"/>
-      <c r="G33"/>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E34" s="2"/>
-      <c r="G34"/>
-      <c r="H34" s="2"/>
-    </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E35" s="2"/>
-      <c r="G35"/>
-      <c r="H35" s="2"/>
-    </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39"/>
-    </row>
-    <row r="40" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40"/>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37"/>
+    </row>
+    <row r="51" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+    </row>
+    <row r="66" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+    </row>
+    <row r="67" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+    </row>
+    <row r="68" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+    </row>
+    <row r="69" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -9017,10 +8798,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -9049,10 +8830,10 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:B22"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9138,41 +8919,41 @@
         <v>54</v>
       </c>
       <c r="T1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="28">
+        <v>3</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="31">
-        <v>3</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="34">
-        <v>0</v>
-      </c>
-      <c r="D2" s="34">
+      <c r="C2" s="31">
+        <v>0</v>
+      </c>
+      <c r="D2" s="31">
         <v>99</v>
       </c>
-      <c r="E2" s="34">
+      <c r="E2" s="31">
         <v>281</v>
       </c>
-      <c r="F2" s="34">
+      <c r="F2" s="31">
         <v>100</v>
       </c>
-      <c r="G2" s="34">
-        <v>0</v>
-      </c>
-      <c r="H2" s="34">
-        <v>0</v>
-      </c>
-      <c r="I2" s="34">
+      <c r="G2" s="31">
+        <v>0</v>
+      </c>
+      <c r="H2" s="31">
+        <v>0</v>
+      </c>
+      <c r="I2" s="31">
         <v>0</v>
       </c>
       <c r="J2" s="2">
         <v>0</v>
       </c>
-      <c r="K2" s="31">
+      <c r="K2" s="28">
         <v>0</v>
       </c>
       <c r="L2" s="2">
@@ -9204,31 +8985,31 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="31">
+      <c r="A3" s="28">
         <v>4</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="34">
-        <v>0</v>
-      </c>
-      <c r="D3" s="34">
+      <c r="B3" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="31">
+        <v>0</v>
+      </c>
+      <c r="D3" s="31">
         <v>91</v>
       </c>
-      <c r="E3" s="34">
+      <c r="E3" s="31">
         <v>9.8000000000000007</v>
       </c>
-      <c r="F3" s="35">
+      <c r="F3" s="32">
         <v>27</v>
       </c>
-      <c r="G3" s="35">
+      <c r="G3" s="32">
         <v>11</v>
       </c>
-      <c r="H3" s="34">
+      <c r="H3" s="31">
         <v>7.93</v>
       </c>
-      <c r="I3" s="34">
+      <c r="I3" s="31">
         <v>0</v>
       </c>
       <c r="J3" s="2">
@@ -9266,31 +9047,31 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="31">
+      <c r="A4" s="28">
         <v>5</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="34">
-        <v>0</v>
-      </c>
-      <c r="D4" s="34">
+        <v>119</v>
+      </c>
+      <c r="C4" s="31">
+        <v>0</v>
+      </c>
+      <c r="D4" s="31">
         <v>89.6</v>
       </c>
-      <c r="E4" s="34">
+      <c r="E4" s="31">
         <v>24</v>
       </c>
-      <c r="F4" s="34">
+      <c r="F4" s="31">
         <v>54</v>
       </c>
-      <c r="G4" s="34">
+      <c r="G4" s="31">
         <v>3.8</v>
       </c>
-      <c r="H4" s="34">
+      <c r="H4" s="31">
         <v>13.06</v>
       </c>
-      <c r="I4" s="34">
+      <c r="I4" s="31">
         <v>0</v>
       </c>
       <c r="J4" s="2">
@@ -9328,31 +9109,31 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="31">
+      <c r="A5" s="28">
         <v>6</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" s="34">
-        <v>0</v>
-      </c>
-      <c r="D5" s="34">
+        <v>120</v>
+      </c>
+      <c r="C5" s="31">
+        <v>0</v>
+      </c>
+      <c r="D5" s="31">
         <v>92.7</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="31">
         <v>65.5</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="31">
         <v>6.4</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="31">
         <v>3.9</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="31">
         <v>1.58</v>
       </c>
-      <c r="I5" s="34">
+      <c r="I5" s="31">
         <v>0</v>
       </c>
       <c r="J5" s="2">
@@ -9390,31 +9171,31 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="31">
+      <c r="A6" s="28">
         <v>7</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="C6" s="34">
-        <v>0</v>
-      </c>
-      <c r="D6" s="34">
+        <v>121</v>
+      </c>
+      <c r="C6" s="31">
+        <v>0</v>
+      </c>
+      <c r="D6" s="31">
         <v>89</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="31">
         <v>3.1</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="31">
         <v>25</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="31">
         <v>5</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="31">
         <v>4.3</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="31">
         <v>0</v>
       </c>
       <c r="J6" s="2">
@@ -9452,31 +9233,31 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="31">
+      <c r="A7" s="28">
         <v>8</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="C7" s="34">
-        <v>0</v>
-      </c>
-      <c r="D7" s="34">
+        <v>122</v>
+      </c>
+      <c r="C7" s="31">
+        <v>0</v>
+      </c>
+      <c r="D7" s="31">
         <v>75</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="31">
         <v>8.5</v>
       </c>
-      <c r="F7" s="34">
+      <c r="F7" s="31">
         <v>100</v>
       </c>
-      <c r="G7" s="34">
-        <v>0</v>
-      </c>
-      <c r="H7" s="34">
+      <c r="G7" s="31">
+        <v>0</v>
+      </c>
+      <c r="H7" s="31">
         <v>70</v>
       </c>
-      <c r="I7" s="34">
+      <c r="I7" s="31">
         <v>4</v>
       </c>
       <c r="J7" s="2">
@@ -9514,31 +9295,31 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="31">
+      <c r="A8" s="28">
         <v>9</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="34">
-        <v>0</v>
-      </c>
-      <c r="D8" s="34">
+        <v>123</v>
+      </c>
+      <c r="C8" s="31">
+        <v>0</v>
+      </c>
+      <c r="D8" s="31">
         <v>90.1</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="31">
         <v>41.5</v>
       </c>
-      <c r="F8" s="34">
+      <c r="F8" s="31">
         <v>30</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="31">
         <v>6.2</v>
       </c>
-      <c r="H8" s="34">
+      <c r="H8" s="31">
         <v>10.34</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="31">
         <v>0</v>
       </c>
       <c r="J8" s="2">
@@ -9576,31 +9357,31 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
+      <c r="A9" s="28">
         <v>10</v>
       </c>
-      <c r="B9" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="C9" s="34">
-        <v>0</v>
-      </c>
-      <c r="D9" s="34">
+      <c r="B9" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="31">
+        <v>0</v>
+      </c>
+      <c r="D9" s="31">
         <v>99</v>
       </c>
-      <c r="E9" s="34">
-        <v>0</v>
-      </c>
-      <c r="F9" s="34">
-        <v>0</v>
-      </c>
-      <c r="G9" s="34">
-        <v>0</v>
-      </c>
-      <c r="H9" s="34">
-        <v>0</v>
-      </c>
-      <c r="I9" s="34">
+      <c r="E9" s="31">
+        <v>0</v>
+      </c>
+      <c r="F9" s="31">
+        <v>0</v>
+      </c>
+      <c r="G9" s="31">
+        <v>0</v>
+      </c>
+      <c r="H9" s="31">
+        <v>0</v>
+      </c>
+      <c r="I9" s="31">
         <v>0</v>
       </c>
       <c r="J9" s="2">
@@ -9638,31 +9419,31 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="31">
+      <c r="A10" s="28">
         <v>11</v>
       </c>
-      <c r="B10" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="C10" s="34">
-        <v>0</v>
-      </c>
-      <c r="D10" s="34">
+      <c r="B10" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="31">
+        <v>0</v>
+      </c>
+      <c r="D10" s="31">
         <v>93.6</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="31">
         <v>42.79</v>
       </c>
-      <c r="F10" s="34">
+      <c r="F10" s="31">
         <v>8</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="31">
         <v>3</v>
       </c>
-      <c r="H10" s="34">
+      <c r="H10" s="31">
         <v>13.5</v>
       </c>
-      <c r="I10" s="34">
+      <c r="I10" s="31">
         <v>0</v>
       </c>
       <c r="J10" s="2">
@@ -9700,37 +9481,37 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="31">
+      <c r="A11" s="28">
         <v>12</v>
       </c>
-      <c r="B11" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="34">
-        <v>0</v>
-      </c>
-      <c r="D11" s="34">
+      <c r="B11" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="31">
+        <v>0</v>
+      </c>
+      <c r="D11" s="31">
         <v>93</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="31">
         <v>26.3</v>
       </c>
-      <c r="F11" s="34">
+      <c r="F11" s="31">
         <v>33.75</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="31">
         <v>6.2</v>
       </c>
-      <c r="H11" s="34">
+      <c r="H11" s="31">
         <v>10.119999999999999</v>
       </c>
-      <c r="I11" s="34">
+      <c r="I11" s="31">
         <v>0</v>
       </c>
       <c r="J11" s="2">
         <v>2.6</v>
       </c>
-      <c r="K11" s="31">
+      <c r="K11" s="28">
         <v>3.0800000000000001E-2</v>
       </c>
       <c r="L11" s="2">
@@ -9762,31 +9543,31 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="31">
+      <c r="A12" s="28">
         <v>16</v>
       </c>
-      <c r="B12" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" s="34">
-        <v>0</v>
-      </c>
-      <c r="D12" s="34">
+      <c r="B12" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="31">
+        <v>0</v>
+      </c>
+      <c r="D12" s="31">
         <v>99</v>
       </c>
-      <c r="E12" s="34">
-        <v>0</v>
-      </c>
-      <c r="F12" s="34">
-        <v>0</v>
-      </c>
-      <c r="G12" s="34">
-        <v>0</v>
-      </c>
-      <c r="H12" s="34">
-        <v>0</v>
-      </c>
-      <c r="I12" s="34">
+      <c r="E12" s="31">
+        <v>0</v>
+      </c>
+      <c r="F12" s="31">
+        <v>0</v>
+      </c>
+      <c r="G12" s="31">
+        <v>0</v>
+      </c>
+      <c r="H12" s="31">
+        <v>0</v>
+      </c>
+      <c r="I12" s="31">
         <v>0</v>
       </c>
       <c r="J12" s="2">
@@ -9824,31 +9605,31 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="31">
+      <c r="A13" s="28">
         <v>17</v>
       </c>
-      <c r="B13" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="C13" s="34">
-        <v>0</v>
-      </c>
-      <c r="D13" s="34">
+      <c r="B13" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="31">
+        <v>0</v>
+      </c>
+      <c r="D13" s="31">
         <v>88.7</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="31">
         <v>17</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="31">
         <v>41</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="31">
         <v>4</v>
       </c>
-      <c r="H13" s="34">
+      <c r="H13" s="31">
         <v>4.7300000000000004</v>
       </c>
-      <c r="I13" s="34">
+      <c r="I13" s="31">
         <v>0</v>
       </c>
       <c r="J13" s="2">
@@ -9886,31 +9667,31 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="31">
+      <c r="A14" s="28">
         <v>18</v>
       </c>
-      <c r="B14" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" s="34">
-        <v>0</v>
-      </c>
-      <c r="D14" s="34">
+      <c r="B14" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="31">
+        <v>0</v>
+      </c>
+      <c r="D14" s="31">
         <v>92.6</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="31">
         <v>29</v>
       </c>
-      <c r="F14" s="34">
+      <c r="F14" s="31">
         <v>4.5</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="31">
         <v>9.86</v>
       </c>
-      <c r="H14" s="34">
+      <c r="H14" s="31">
         <v>2.62</v>
       </c>
-      <c r="I14" s="34">
+      <c r="I14" s="31">
         <v>0</v>
       </c>
       <c r="J14" s="2">
@@ -9948,31 +9729,31 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="31">
+      <c r="A15" s="28">
         <v>19</v>
       </c>
-      <c r="B15" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="C15" s="34">
-        <v>0</v>
-      </c>
-      <c r="D15" s="34">
+      <c r="B15" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="31">
+        <v>0</v>
+      </c>
+      <c r="D15" s="31">
         <v>95</v>
       </c>
-      <c r="E15" s="34">
+      <c r="E15" s="31">
         <v>10</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="31">
         <v>25</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="31">
         <v>0.8</v>
       </c>
-      <c r="H15" s="34">
+      <c r="H15" s="31">
         <v>1.6</v>
       </c>
-      <c r="I15" s="34">
+      <c r="I15" s="31">
         <v>0</v>
       </c>
       <c r="J15" s="2">
@@ -10010,31 +9791,31 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="31">
+      <c r="A16" s="28">
         <v>20</v>
       </c>
-      <c r="B16" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="C16" s="34">
-        <v>0</v>
-      </c>
-      <c r="D16" s="34">
+      <c r="B16" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="31">
+        <v>0</v>
+      </c>
+      <c r="D16" s="31">
         <v>88.5</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E16" s="31">
         <v>20.100000000000001</v>
       </c>
-      <c r="F16" s="34">
+      <c r="F16" s="31">
         <v>44</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="31">
         <v>1.49</v>
       </c>
-      <c r="H16" s="34">
+      <c r="H16" s="31">
         <v>5.59</v>
       </c>
-      <c r="I16" s="34">
+      <c r="I16" s="31">
         <v>0</v>
       </c>
       <c r="J16" s="2">
@@ -10072,31 +9853,31 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="31">
+      <c r="A17" s="28">
         <v>21</v>
       </c>
-      <c r="B17" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="C17" s="34">
-        <v>0</v>
-      </c>
-      <c r="D17" s="34">
+      <c r="B17" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="31">
+        <v>0</v>
+      </c>
+      <c r="D17" s="31">
         <v>89</v>
       </c>
-      <c r="E17" s="34">
+      <c r="E17" s="31">
         <v>18.39</v>
       </c>
-      <c r="F17" s="34">
+      <c r="F17" s="31">
         <v>40</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="31">
         <v>3</v>
       </c>
-      <c r="H17" s="34">
+      <c r="H17" s="31">
         <v>3.94</v>
       </c>
-      <c r="I17" s="34">
+      <c r="I17" s="31">
         <v>0</v>
       </c>
       <c r="J17" s="2">
@@ -10134,31 +9915,31 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="31">
+      <c r="A18" s="28">
         <v>25</v>
       </c>
-      <c r="B18" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="C18" s="34">
+      <c r="B18" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="31">
         <v>100</v>
       </c>
-      <c r="D18" s="37">
+      <c r="D18" s="34">
         <v>89</v>
       </c>
-      <c r="E18" s="37">
+      <c r="E18" s="34">
         <v>10</v>
       </c>
-      <c r="F18" s="38">
+      <c r="F18" s="35">
         <v>38</v>
       </c>
-      <c r="G18" s="38">
+      <c r="G18" s="35">
         <v>6.09</v>
       </c>
-      <c r="H18" s="38">
+      <c r="H18" s="35">
         <v>5.09</v>
       </c>
-      <c r="I18" s="38">
+      <c r="I18" s="35">
         <v>1</v>
       </c>
       <c r="J18" s="2">
@@ -10196,31 +9977,31 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="31">
+      <c r="A19" s="28">
         <v>28</v>
       </c>
-      <c r="B19" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="C19" s="34">
-        <v>0</v>
-      </c>
-      <c r="D19" s="34">
+      <c r="B19" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="31">
+        <v>0</v>
+      </c>
+      <c r="D19" s="31">
         <v>93</v>
       </c>
-      <c r="E19" s="34">
+      <c r="E19" s="31">
         <v>40.200000000000003</v>
       </c>
-      <c r="F19" s="34">
+      <c r="F19" s="31">
         <v>33.79</v>
       </c>
-      <c r="G19" s="34">
+      <c r="G19" s="31">
         <v>6.2</v>
       </c>
-      <c r="H19" s="34">
+      <c r="H19" s="31">
         <v>5.88</v>
       </c>
-      <c r="I19" s="34">
+      <c r="I19" s="31">
         <v>0</v>
       </c>
       <c r="J19" s="2">
@@ -10258,31 +10039,31 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="31">
+      <c r="A20" s="28">
         <v>29</v>
       </c>
-      <c r="B20" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="C20" s="34">
-        <v>0</v>
-      </c>
-      <c r="D20" s="34">
+      <c r="B20" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" s="31">
+        <v>0</v>
+      </c>
+      <c r="D20" s="31">
         <v>93</v>
       </c>
-      <c r="E20" s="34">
+      <c r="E20" s="31">
         <v>48.89</v>
       </c>
-      <c r="F20" s="34">
+      <c r="F20" s="31">
         <v>33.79</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="31">
         <v>6.2</v>
       </c>
-      <c r="H20" s="34">
+      <c r="H20" s="31">
         <v>4.3</v>
       </c>
-      <c r="I20" s="34">
+      <c r="I20" s="31">
         <v>0</v>
       </c>
       <c r="J20" s="2">
@@ -10320,37 +10101,37 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="31">
+      <c r="A21" s="28">
         <v>30</v>
       </c>
-      <c r="B21" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="C21" s="34">
+      <c r="B21" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="C21" s="31">
         <v>100</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D21" s="31">
         <v>35</v>
       </c>
-      <c r="E21" s="34">
+      <c r="E21" s="31">
         <v>8</v>
       </c>
-      <c r="F21" s="34">
+      <c r="F21" s="31">
         <v>50</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="31">
         <v>4.8499999999999996</v>
       </c>
-      <c r="H21" s="34">
+      <c r="H21" s="31">
         <v>0.89</v>
       </c>
-      <c r="I21" s="34">
+      <c r="I21" s="31">
         <v>0</v>
       </c>
       <c r="J21" s="2">
         <v>3.18</v>
       </c>
-      <c r="K21" s="31">
+      <c r="K21" s="28">
         <v>6.0479999999999999E-2</v>
       </c>
       <c r="L21" s="2">
@@ -10382,31 +10163,31 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="31">
+      <c r="A22" s="28">
         <v>31</v>
       </c>
-      <c r="B22" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="C22" s="34">
+      <c r="B22" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="31">
         <v>100</v>
       </c>
-      <c r="D22" s="34">
+      <c r="D22" s="31">
         <v>35</v>
       </c>
-      <c r="E22" s="34">
+      <c r="E22" s="31">
         <v>14.69</v>
       </c>
-      <c r="F22" s="34">
+      <c r="F22" s="31">
         <v>55</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="31">
         <v>6</v>
       </c>
-      <c r="H22" s="34">
+      <c r="H22" s="31">
         <v>3.34</v>
       </c>
-      <c r="I22" s="34">
+      <c r="I22" s="31">
         <v>0</v>
       </c>
       <c r="J22" s="2">
@@ -10444,42 +10225,42 @@
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B41" s="31"/>
-      <c r="Q41" s="31"/>
+      <c r="B41" s="28"/>
+      <c r="Q41" s="28"/>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B42" s="31"/>
-      <c r="Q42" s="31"/>
+      <c r="B42" s="28"/>
+      <c r="Q42" s="28"/>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B43" s="31"/>
-      <c r="Q43" s="31"/>
+      <c r="B43" s="28"/>
+      <c r="Q43" s="28"/>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B44" s="31"/>
-      <c r="Q44" s="31"/>
+      <c r="B44" s="28"/>
+      <c r="Q44" s="28"/>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B45" s="31"/>
-      <c r="Q45" s="50"/>
+      <c r="B45" s="28"/>
+      <c r="Q45" s="47"/>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B46" s="31"/>
+      <c r="B46" s="28"/>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B47" s="31"/>
+      <c r="B47" s="28"/>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B48" s="31"/>
+      <c r="B48" s="28"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="31"/>
+      <c r="B49" s="28"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="31"/>
+      <c r="B50" s="28"/>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="31"/>
+      <c r="B51" s="28"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B19 B2:I18">
@@ -10511,7 +10292,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D20"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10524,52 +10305,52 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
-        <v>117</v>
+      <c r="A2" s="48" t="s">
+        <v>114</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="27">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
-        <v>121</v>
+      <c r="A3" s="36" t="s">
+        <v>118</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C3" s="2">
         <v>4</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="27">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>122</v>
+      <c r="A4" s="29" t="s">
+        <v>119</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C4" s="2">
         <v>5</v>
@@ -10579,11 +10360,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
-        <v>123</v>
+      <c r="A5" s="29" t="s">
+        <v>120</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C5" s="2">
         <v>6</v>
@@ -10593,11 +10374,11 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
-        <v>124</v>
+      <c r="A6" s="29" t="s">
+        <v>121</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C6" s="2">
         <v>7</v>
@@ -10607,11 +10388,11 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
-        <v>125</v>
+      <c r="A7" s="29" t="s">
+        <v>122</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C7" s="2">
         <v>8</v>
@@ -10621,165 +10402,165 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
-        <v>126</v>
+      <c r="A8" s="29" t="s">
+        <v>123</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C8" s="2">
         <v>9</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="27">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
-        <v>127</v>
+      <c r="A9" s="36" t="s">
+        <v>124</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C9" s="2">
         <v>10</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="27">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
-        <v>128</v>
+      <c r="A10" s="36" t="s">
+        <v>125</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C10" s="2">
         <v>11</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="27">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
-        <v>130</v>
+      <c r="A11" s="36" t="s">
+        <v>127</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C11" s="2">
         <v>12</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="27">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
-        <v>132</v>
+      <c r="A12" s="36" t="s">
+        <v>129</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C12" s="2">
         <v>16</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="27">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
-        <v>133</v>
+      <c r="A13" s="36" t="s">
+        <v>130</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C13" s="2">
         <v>17</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="27">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
-        <v>134</v>
+      <c r="A14" s="36" t="s">
+        <v>131</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C14" s="2">
         <v>18</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="27">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
-        <v>135</v>
+      <c r="A15" s="36" t="s">
+        <v>132</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C15" s="2">
         <v>19</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="27">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
-        <v>136</v>
+      <c r="A16" s="36" t="s">
+        <v>133</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C16" s="2">
         <v>20</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="27">
         <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
-        <v>137</v>
+      <c r="A17" s="36" t="s">
+        <v>134</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C17" s="2">
         <v>21</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="27">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="52" t="s">
-        <v>139</v>
+      <c r="A18" s="49" t="s">
+        <v>136</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C18" s="2">
         <v>25</v>
       </c>
-      <c r="D18" s="49">
+      <c r="D18" s="46">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
-        <v>129</v>
+      <c r="A19" s="36" t="s">
+        <v>126</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C19" s="2">
         <v>28</v>
@@ -10789,11 +10570,11 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
-        <v>131</v>
+      <c r="A20" s="36" t="s">
+        <v>128</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C20" s="2">
         <v>29</v>
@@ -10803,22 +10584,22 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
-        <v>160</v>
+      <c r="A21" s="36" t="s">
+        <v>157</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C21" s="2">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="55" t="s">
-        <v>138</v>
+      <c r="A22" s="52" t="s">
+        <v>135</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C22" s="2">
         <v>31</v>
@@ -10848,43 +10629,43 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:J5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="24.42578125" style="24"/>
+    <col min="1" max="16384" width="24.42578125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:10" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="F1" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="61" t="s">
+      <c r="H1" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="61" t="s">
+      <c r="J1" s="58" t="s">
         <v>102</v>
       </c>
     </row>
@@ -11033,13 +10814,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="C6">
-        <v>0.2</v>
-      </c>
-      <c r="D6">
-        <v>0.4</v>
+        <v>0.15</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.55000000000000004</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -11047,8 +10828,8 @@
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6">
-        <v>0.2</v>
+      <c r="G6" s="2">
+        <v>0.15</v>
       </c>
       <c r="H6" t="s">
         <v>103</v>
@@ -11056,8 +10837,8 @@
       <c r="I6" t="s">
         <v>103</v>
       </c>
-      <c r="J6" t="b">
-        <v>0</v>
+      <c r="J6" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -11075,588 +10856,593 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E5" sqref="E5:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="21.7109375" style="25"/>
-    <col min="9" max="9" width="21.7109375" style="25" customWidth="1"/>
-    <col min="10" max="16384" width="21.7109375" style="25"/>
+    <col min="1" max="1" width="5" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="24" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="24" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="24" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="24" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="24" customWidth="1"/>
+    <col min="10" max="16384" width="21.7109375" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="28" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:8" s="25" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="45" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="27">
+        <v>21</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="55">
+        <v>6.0269407000000002E-4</v>
+      </c>
+      <c r="D2" s="55">
+        <v>0.82331812000000004</v>
+      </c>
+      <c r="E2" s="55">
+        <v>9.2401000999999996E-2</v>
+      </c>
+      <c r="F2" s="55">
+        <v>2.2715029999999998E-3</v>
+      </c>
+      <c r="G2" s="55">
+        <v>8.7793080999999998E-4</v>
+      </c>
+      <c r="H2" s="55">
+        <v>0.29167724</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>8</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="56">
+        <v>3.0914954E-4</v>
+      </c>
+      <c r="D3" s="56">
+        <v>1.38809</v>
+      </c>
+      <c r="E3" s="56">
+        <v>9.5984228000000005E-2</v>
+      </c>
+      <c r="F3" s="56">
+        <v>1.4925155E-3</v>
+      </c>
+      <c r="G3" s="56">
+        <v>5.9082242000000002E-4</v>
+      </c>
+      <c r="H3" s="56">
+        <v>0.25908868000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27">
+        <v>19</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="55">
+        <v>6.8793711999999996E-4</v>
+      </c>
+      <c r="D4" s="55">
+        <v>0.93976550999999997</v>
+      </c>
+      <c r="E4" s="55">
+        <v>0.10546989</v>
+      </c>
+      <c r="F4" s="55">
+        <v>2.5927768E-3</v>
+      </c>
+      <c r="G4" s="55">
+        <v>1.0021024000000001E-3</v>
+      </c>
+      <c r="H4" s="55">
+        <v>0.33293109999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27">
+        <v>31</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="56">
+        <v>1.398646E-5</v>
+      </c>
+      <c r="D5" s="56">
+        <v>1.0869945000000001</v>
+      </c>
+      <c r="E5" s="56">
+        <v>0.18026732000000001</v>
+      </c>
+      <c r="F5" s="56">
+        <v>7.1452427000000002E-3</v>
+      </c>
+      <c r="G5" s="56">
+        <v>1.8322938999999999E-3</v>
+      </c>
+      <c r="H5" s="56">
+        <v>1.1594272000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="53">
+        <v>30</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="57">
+        <v>1.4238930000000001E-3</v>
+      </c>
+      <c r="D6" s="57">
+        <v>1.2922062999999999</v>
+      </c>
+      <c r="E6" s="57">
+        <v>0.19672819999999999</v>
+      </c>
+      <c r="F6" s="57">
+        <v>8.0315088999999996E-3</v>
+      </c>
+      <c r="G6" s="57">
+        <v>2.7384863000000001E-3</v>
+      </c>
+      <c r="H6" s="57">
+        <v>0.89059001000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27">
+        <v>12</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="55">
+        <v>1.8296865E-3</v>
+      </c>
+      <c r="D7" s="55">
+        <v>2.1376919999999999</v>
+      </c>
+      <c r="E7" s="55">
+        <v>0.21715095000000001</v>
+      </c>
+      <c r="F7" s="55">
+        <v>3.8183357999999998E-3</v>
+      </c>
+      <c r="G7" s="55">
+        <v>3.2683618999999999E-3</v>
+      </c>
+      <c r="H7" s="55">
+        <v>1.6645894999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27">
+        <v>25</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="56">
+        <v>1.4474578E-5</v>
+      </c>
+      <c r="D8" s="56">
+        <v>2.1134135000000001</v>
+      </c>
+      <c r="E8" s="56">
+        <v>0.22375627000000001</v>
+      </c>
+      <c r="F8" s="56">
+        <v>7.2554300000000002E-3</v>
+      </c>
+      <c r="G8" s="56">
+        <v>1.8719005000000001E-3</v>
+      </c>
+      <c r="H8" s="56">
+        <v>1.1395907999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
+        <v>5</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="56">
+        <v>9.8875607000000008E-4</v>
+      </c>
+      <c r="D9" s="56">
+        <v>3.4574254999999998</v>
+      </c>
+      <c r="E9" s="56">
+        <v>0.22933355999999999</v>
+      </c>
+      <c r="F9" s="56">
+        <v>4.8724891000000003E-3</v>
+      </c>
+      <c r="G9" s="56">
+        <v>1.5442412000000001E-3</v>
+      </c>
+      <c r="H9" s="56">
+        <v>0.43937693999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27">
+        <v>4</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="56">
+        <v>6.5774577999999997E-4</v>
+      </c>
+      <c r="D10" s="56">
+        <v>5.2727627000000004</v>
+      </c>
+      <c r="E10" s="56">
+        <v>0.23187210999999999</v>
+      </c>
+      <c r="F10" s="56">
+        <v>3.2484240000000002E-3</v>
+      </c>
+      <c r="G10" s="56">
+        <v>1.2782201999999999E-3</v>
+      </c>
+      <c r="H10" s="56">
+        <v>0.55197054999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27">
+        <v>28</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="56">
+        <v>2.1675339E-3</v>
+      </c>
+      <c r="D11" s="56">
+        <v>2.3852028000000001</v>
+      </c>
+      <c r="E11" s="56">
+        <v>0.24039757</v>
+      </c>
+      <c r="F11" s="56">
+        <v>4.5559939999999998E-3</v>
+      </c>
+      <c r="G11" s="56">
+        <v>3.8858629999999998E-3</v>
+      </c>
+      <c r="H11" s="56">
+        <v>1.9759963</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27">
+        <v>29</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="55">
+        <v>2.1675339E-3</v>
+      </c>
+      <c r="D12" s="55">
+        <v>2.3852028000000001</v>
+      </c>
+      <c r="E12" s="55">
+        <v>0.24039757</v>
+      </c>
+      <c r="F12" s="55">
+        <v>4.5559939999999998E-3</v>
+      </c>
+      <c r="G12" s="55">
+        <v>3.8858629999999998E-3</v>
+      </c>
+      <c r="H12" s="55">
+        <v>1.9759963</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
+        <v>7</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="56">
+        <v>5.2979589999999997E-3</v>
+      </c>
+      <c r="D13" s="56">
+        <v>2.6504308999999999</v>
+      </c>
+      <c r="E13" s="56">
+        <v>0.25521818000000002</v>
+      </c>
+      <c r="F13" s="56">
+        <v>2.7713717000000001E-3</v>
+      </c>
+      <c r="G13" s="56">
+        <v>4.3737089999999999E-3</v>
+      </c>
+      <c r="H13" s="56">
+        <v>2.4169052999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27">
+        <v>11</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="55">
+        <v>3.8977495E-3</v>
+      </c>
+      <c r="D14" s="55">
+        <v>6.6378231000000003</v>
+      </c>
+      <c r="E14" s="55">
+        <v>0.33354636999999998</v>
+      </c>
+      <c r="F14" s="55">
+        <v>3.6638446000000001E-3</v>
+      </c>
+      <c r="G14" s="55">
+        <v>6.3452205000000001E-3</v>
+      </c>
+      <c r="H14" s="55">
+        <v>3.8084742</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="27">
+        <v>17</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="55">
+        <v>1.2856242E-3</v>
+      </c>
+      <c r="D15" s="55">
+        <v>5.4884582999999996</v>
+      </c>
+      <c r="E15" s="55">
+        <v>0.33457320000000002</v>
+      </c>
+      <c r="F15" s="55">
+        <v>5.0812655999999999E-3</v>
+      </c>
+      <c r="G15" s="55">
+        <v>2.1954254000000001E-3</v>
+      </c>
+      <c r="H15" s="55">
+        <v>0.62333822000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17">
+        <v>9</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="56">
+        <v>2.4268531000000001E-3</v>
+      </c>
+      <c r="D16" s="56">
+        <v>2.7512188000000002</v>
+      </c>
+      <c r="E16" s="56">
+        <v>0.37877785000000003</v>
+      </c>
+      <c r="F16" s="56">
+        <v>8.1080295000000007E-3</v>
+      </c>
+      <c r="G16" s="56">
+        <v>3.0197698000000001E-3</v>
+      </c>
+      <c r="H16" s="56">
+        <v>1.2147266999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="27">
+        <v>20</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C17" s="55">
+        <v>1.7751223E-3</v>
+      </c>
+      <c r="D17" s="55">
+        <v>7.5781744</v>
+      </c>
+      <c r="E17" s="55">
+        <v>0.46196108000000002</v>
+      </c>
+      <c r="F17" s="55">
+        <v>7.0159441999999997E-3</v>
+      </c>
+      <c r="G17" s="55">
+        <v>3.0313279000000002E-3</v>
+      </c>
+      <c r="H17" s="55">
+        <v>0.86067262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="27">
+        <v>18</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="55">
+        <v>2.0170432000000001E-3</v>
+      </c>
+      <c r="D18" s="55">
+        <v>9.4737010999999995</v>
+      </c>
+      <c r="E18" s="55">
+        <v>0.57584038999999998</v>
+      </c>
+      <c r="F18" s="55">
+        <v>7.9888571999999995E-3</v>
+      </c>
+      <c r="G18" s="55">
+        <v>6.0113188999999997E-3</v>
+      </c>
+      <c r="H18" s="55">
+        <v>0.97791181999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>6</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="56">
+        <v>4.6734098000000002E-3</v>
+      </c>
+      <c r="D19" s="56">
+        <v>16.341711</v>
+      </c>
+      <c r="E19" s="56">
+        <v>1.0839576</v>
+      </c>
+      <c r="F19" s="56">
+        <v>2.3030087000000001E-2</v>
+      </c>
+      <c r="G19" s="56">
+        <v>7.2989407999999997E-3</v>
+      </c>
+      <c r="H19" s="56">
+        <v>2.0767392</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27">
+        <v>16</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="55">
+        <v>9.5703047000000006E-3</v>
+      </c>
+      <c r="D20" s="55">
+        <v>11.181349000000001</v>
+      </c>
+      <c r="E20" s="55">
+        <v>1.1358234</v>
+      </c>
+      <c r="F20" s="55">
+        <v>1.9972074999999999E-2</v>
+      </c>
+      <c r="G20" s="55">
+        <v>1.7095398000000001E-2</v>
+      </c>
+      <c r="H20" s="55">
+        <v>8.7067530000000009</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="27">
+        <v>10</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" s="55">
+        <v>1.1524281000000001E-2</v>
+      </c>
+      <c r="D21" s="55">
+        <v>13.064581</v>
+      </c>
+      <c r="E21" s="55">
+        <v>1.7986842999999999</v>
+      </c>
+      <c r="F21" s="55">
+        <v>3.8502213E-2</v>
+      </c>
+      <c r="G21" s="55">
+        <v>1.4339836999999999E-2</v>
+      </c>
+      <c r="H21" s="55">
+        <v>5.7683147000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>3</v>
       </c>
-      <c r="B2" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="58">
+      <c r="B22" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="55">
         <v>5.3300000000000001E-5</v>
       </c>
-      <c r="D2" s="58">
+      <c r="D22" s="55">
         <v>67</v>
       </c>
-      <c r="E2" s="58">
+      <c r="E22" s="55">
         <v>3.7</v>
       </c>
-      <c r="F2" s="58">
+      <c r="F22" s="55">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G2" s="58">
+      <c r="G22" s="55">
         <v>4.5599999999999998E-3</v>
       </c>
-      <c r="H2" s="58">
+      <c r="H22" s="55">
         <v>8.2600000000000007E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30">
-        <v>4</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="59">
-        <v>6.5774577999999997E-4</v>
-      </c>
-      <c r="D3" s="59">
-        <v>5.2727627000000004</v>
-      </c>
-      <c r="E3" s="59">
-        <v>0.23187210999999999</v>
-      </c>
-      <c r="F3" s="59">
-        <v>3.2484240000000002E-3</v>
-      </c>
-      <c r="G3" s="59">
-        <v>1.2782201999999999E-3</v>
-      </c>
-      <c r="H3" s="59">
-        <v>0.55197054999999995</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
-        <v>5</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="59">
-        <v>9.8875607000000008E-4</v>
-      </c>
-      <c r="D4" s="59">
-        <v>3.4574254999999998</v>
-      </c>
-      <c r="E4" s="59">
-        <v>0.22933355999999999</v>
-      </c>
-      <c r="F4" s="59">
-        <v>4.8724891000000003E-3</v>
-      </c>
-      <c r="G4" s="59">
-        <v>1.5442412000000001E-3</v>
-      </c>
-      <c r="H4" s="59">
-        <v>0.43937693999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
-        <v>6</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" s="59">
-        <v>4.6734098000000002E-3</v>
-      </c>
-      <c r="D5" s="59">
-        <v>16.341711</v>
-      </c>
-      <c r="E5" s="59">
-        <v>1.0839576</v>
-      </c>
-      <c r="F5" s="59">
-        <v>2.3030087000000001E-2</v>
-      </c>
-      <c r="G5" s="59">
-        <v>7.2989407999999997E-3</v>
-      </c>
-      <c r="H5" s="59">
-        <v>2.0767392</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
-        <v>7</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>124</v>
-      </c>
-      <c r="C6" s="59">
-        <v>5.2979589999999997E-3</v>
-      </c>
-      <c r="D6" s="59">
-        <v>2.6504308999999999</v>
-      </c>
-      <c r="E6" s="59">
-        <v>0.25521818000000002</v>
-      </c>
-      <c r="F6" s="59">
-        <v>2.7713717000000001E-3</v>
-      </c>
-      <c r="G6" s="59">
-        <v>4.3737089999999999E-3</v>
-      </c>
-      <c r="H6" s="59">
-        <v>2.4169052999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
-        <v>8</v>
-      </c>
-      <c r="B7" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="C7" s="59">
-        <v>3.0914954E-4</v>
-      </c>
-      <c r="D7" s="59">
-        <v>1.38809</v>
-      </c>
-      <c r="E7" s="59">
-        <v>9.5984228000000005E-2</v>
-      </c>
-      <c r="F7" s="59">
-        <v>1.4925155E-3</v>
-      </c>
-      <c r="G7" s="59">
-        <v>5.9082242000000002E-4</v>
-      </c>
-      <c r="H7" s="59">
-        <v>0.25908868000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
-        <v>9</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="59">
-        <v>2.4268531000000001E-3</v>
-      </c>
-      <c r="D8" s="59">
-        <v>2.7512188000000002</v>
-      </c>
-      <c r="E8" s="59">
-        <v>0.37877785000000003</v>
-      </c>
-      <c r="F8" s="59">
-        <v>8.1080295000000007E-3</v>
-      </c>
-      <c r="G8" s="59">
-        <v>3.0197698000000001E-3</v>
-      </c>
-      <c r="H8" s="59">
-        <v>1.2147266999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30">
-        <v>10</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>127</v>
-      </c>
-      <c r="C9" s="58">
-        <v>1.1524281000000001E-2</v>
-      </c>
-      <c r="D9" s="58">
-        <v>13.064581</v>
-      </c>
-      <c r="E9" s="58">
-        <v>1.7986842999999999</v>
-      </c>
-      <c r="F9" s="58">
-        <v>3.8502213E-2</v>
-      </c>
-      <c r="G9" s="58">
-        <v>1.4339836999999999E-2</v>
-      </c>
-      <c r="H9" s="58">
-        <v>5.7683147000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30">
-        <v>11</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>128</v>
-      </c>
-      <c r="C10" s="58">
-        <v>3.8977495E-3</v>
-      </c>
-      <c r="D10" s="58">
-        <v>6.6378231000000003</v>
-      </c>
-      <c r="E10" s="58">
-        <v>0.33354636999999998</v>
-      </c>
-      <c r="F10" s="58">
-        <v>3.6638446000000001E-3</v>
-      </c>
-      <c r="G10" s="58">
-        <v>6.3452205000000001E-3</v>
-      </c>
-      <c r="H10" s="58">
-        <v>3.8084742</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30">
-        <v>28</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="59">
-        <v>2.1675339E-3</v>
-      </c>
-      <c r="D11" s="59">
-        <v>2.3852028000000001</v>
-      </c>
-      <c r="E11" s="59">
-        <v>0.24039757</v>
-      </c>
-      <c r="F11" s="59">
-        <v>4.5559939999999998E-3</v>
-      </c>
-      <c r="G11" s="59">
-        <v>3.8858629999999998E-3</v>
-      </c>
-      <c r="H11" s="59">
-        <v>1.9759963</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30">
-        <v>12</v>
-      </c>
-      <c r="B12" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" s="58">
-        <v>1.8296865E-3</v>
-      </c>
-      <c r="D12" s="58">
-        <v>2.1376919999999999</v>
-      </c>
-      <c r="E12" s="58">
-        <v>0.21715095000000001</v>
-      </c>
-      <c r="F12" s="58">
-        <v>3.8183357999999998E-3</v>
-      </c>
-      <c r="G12" s="58">
-        <v>3.2683618999999999E-3</v>
-      </c>
-      <c r="H12" s="58">
-        <v>1.6645894999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30">
-        <v>29</v>
-      </c>
-      <c r="B13" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" s="58">
-        <v>2.1675339E-3</v>
-      </c>
-      <c r="D13" s="58">
-        <v>2.3852028000000001</v>
-      </c>
-      <c r="E13" s="58">
-        <v>0.24039757</v>
-      </c>
-      <c r="F13" s="58">
-        <v>4.5559939999999998E-3</v>
-      </c>
-      <c r="G13" s="58">
-        <v>3.8858629999999998E-3</v>
-      </c>
-      <c r="H13" s="58">
-        <v>1.9759963</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30">
-        <v>16</v>
-      </c>
-      <c r="B14" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="C14" s="58">
-        <v>9.5703047000000006E-3</v>
-      </c>
-      <c r="D14" s="58">
-        <v>11.181349000000001</v>
-      </c>
-      <c r="E14" s="58">
-        <v>1.1358234</v>
-      </c>
-      <c r="F14" s="58">
-        <v>1.9972074999999999E-2</v>
-      </c>
-      <c r="G14" s="58">
-        <v>1.7095398000000001E-2</v>
-      </c>
-      <c r="H14" s="58">
-        <v>8.7067530000000009</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="30">
-        <v>17</v>
-      </c>
-      <c r="B15" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="58">
-        <v>1.2856242E-3</v>
-      </c>
-      <c r="D15" s="58">
-        <v>5.4884582999999996</v>
-      </c>
-      <c r="E15" s="58">
-        <v>0.33457320000000002</v>
-      </c>
-      <c r="F15" s="58">
-        <v>5.0812655999999999E-3</v>
-      </c>
-      <c r="G15" s="58">
-        <v>2.1954254000000001E-3</v>
-      </c>
-      <c r="H15" s="58">
-        <v>0.62333822000000005</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30">
-        <v>18</v>
-      </c>
-      <c r="B16" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="C16" s="58">
-        <v>2.0170432000000001E-3</v>
-      </c>
-      <c r="D16" s="58">
-        <v>9.4737010999999995</v>
-      </c>
-      <c r="E16" s="58">
-        <v>0.57584038999999998</v>
-      </c>
-      <c r="F16" s="58">
-        <v>7.9888571999999995E-3</v>
-      </c>
-      <c r="G16" s="58">
-        <v>6.0113188999999997E-3</v>
-      </c>
-      <c r="H16" s="58">
-        <v>0.97791181999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30">
-        <v>19</v>
-      </c>
-      <c r="B17" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="C17" s="58">
-        <v>6.8793711999999996E-4</v>
-      </c>
-      <c r="D17" s="58">
-        <v>0.93976550999999997</v>
-      </c>
-      <c r="E17" s="58">
-        <v>0.10546989</v>
-      </c>
-      <c r="F17" s="58">
-        <v>2.5927768E-3</v>
-      </c>
-      <c r="G17" s="58">
-        <v>1.0021024000000001E-3</v>
-      </c>
-      <c r="H17" s="58">
-        <v>0.33293109999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30">
-        <v>20</v>
-      </c>
-      <c r="B18" s="40" t="s">
-        <v>136</v>
-      </c>
-      <c r="C18" s="58">
-        <v>1.7751223E-3</v>
-      </c>
-      <c r="D18" s="58">
-        <v>7.5781744</v>
-      </c>
-      <c r="E18" s="58">
-        <v>0.46196108000000002</v>
-      </c>
-      <c r="F18" s="58">
-        <v>7.0159441999999997E-3</v>
-      </c>
-      <c r="G18" s="58">
-        <v>3.0313279000000002E-3</v>
-      </c>
-      <c r="H18" s="58">
-        <v>0.86067262</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30">
-        <v>21</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="C19" s="58">
-        <v>6.0269407000000002E-4</v>
-      </c>
-      <c r="D19" s="58">
-        <v>0.82331812000000004</v>
-      </c>
-      <c r="E19" s="58">
-        <v>9.2401000999999996E-2</v>
-      </c>
-      <c r="F19" s="58">
-        <v>2.2715029999999998E-3</v>
-      </c>
-      <c r="G19" s="58">
-        <v>8.7793080999999998E-4</v>
-      </c>
-      <c r="H19" s="58">
-        <v>0.29167724</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30">
-        <v>31</v>
-      </c>
-      <c r="B20" s="47" t="s">
-        <v>138</v>
-      </c>
-      <c r="C20" s="59">
-        <v>1.398646E-5</v>
-      </c>
-      <c r="D20" s="59">
-        <v>1.0869945000000001</v>
-      </c>
-      <c r="E20" s="59">
-        <v>0.18026732000000001</v>
-      </c>
-      <c r="F20" s="59">
-        <v>7.1452427000000002E-3</v>
-      </c>
-      <c r="G20" s="59">
-        <v>1.8322938999999999E-3</v>
-      </c>
-      <c r="H20" s="59">
-        <v>1.1594272000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30">
-        <v>25</v>
-      </c>
-      <c r="B21" s="43" t="s">
-        <v>139</v>
-      </c>
-      <c r="C21" s="59">
-        <v>1.4474578E-5</v>
-      </c>
-      <c r="D21" s="59">
-        <v>2.1134135000000001</v>
-      </c>
-      <c r="E21" s="59">
-        <v>0.22375627000000001</v>
-      </c>
-      <c r="F21" s="59">
-        <v>7.2554300000000002E-3</v>
-      </c>
-      <c r="G21" s="59">
-        <v>1.8719005000000001E-3</v>
-      </c>
-      <c r="H21" s="59">
-        <v>1.1395907999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="56">
-        <v>30</v>
-      </c>
-      <c r="B22" s="57" t="s">
-        <v>160</v>
-      </c>
-      <c r="C22" s="60">
-        <v>1.4238930000000001E-3</v>
-      </c>
-      <c r="D22" s="60">
-        <v>1.2922062999999999</v>
-      </c>
-      <c r="E22" s="60">
-        <v>0.19672819999999999</v>
-      </c>
-      <c r="F22" s="60">
-        <v>8.0315088999999996E-3</v>
-      </c>
-      <c r="G22" s="60">
-        <v>2.7384863000000001E-3</v>
-      </c>
-      <c r="H22" s="60">
-        <v>0.89059001000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Parity with EMB model
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="14490" windowHeight="11160" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="14490" windowHeight="11160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -8211,8 +8211,8 @@
   </sheetPr>
   <dimension ref="A1:X69"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8311,7 +8311,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B2" s="19">
         <v>1</v>
@@ -8347,7 +8347,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="19">
-        <v>8.1999999999999993</v>
+        <v>6.5</v>
       </c>
       <c r="N2" s="20">
         <v>2.41</v>
@@ -8359,10 +8359,10 @@
         <v>161</v>
       </c>
       <c r="Q2" s="19">
-        <v>0.7</v>
+        <v>1.3</v>
       </c>
       <c r="R2" s="19">
-        <v>3</v>
+        <v>1.86</v>
       </c>
       <c r="S2" s="19">
         <v>0.01</v>
@@ -8385,7 +8385,7 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="22">
         <v>1</v>
@@ -8421,7 +8421,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="19">
-        <v>8.1999999999999993</v>
+        <v>6.5</v>
       </c>
       <c r="N3" s="20">
         <v>2.41</v>
@@ -8433,10 +8433,10 @@
         <v>117</v>
       </c>
       <c r="Q3" s="19">
-        <v>1.43</v>
+        <v>1.3</v>
       </c>
       <c r="R3" s="19">
-        <v>2.09</v>
+        <v>1.86</v>
       </c>
       <c r="S3" s="22">
         <v>1E-3</v>
@@ -8495,7 +8495,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="19">
-        <v>8.1999999999999993</v>
+        <v>6.5</v>
       </c>
       <c r="N4" s="20">
         <v>2.41</v>
@@ -8507,10 +8507,10 @@
         <v>110</v>
       </c>
       <c r="Q4" s="19">
-        <v>1.75</v>
+        <v>1.3</v>
       </c>
       <c r="R4" s="19">
-        <v>1.9</v>
+        <v>1.86</v>
       </c>
       <c r="S4" s="22">
         <v>1E-3</v>
@@ -8568,8 +8568,8 @@
       <c r="L5" s="60">
         <v>0</v>
       </c>
-      <c r="M5" s="59">
-        <v>8.1999999999999993</v>
+      <c r="M5" s="19">
+        <v>6.5</v>
       </c>
       <c r="N5" s="62">
         <v>2.41</v>
@@ -8581,10 +8581,10 @@
         <v>110</v>
       </c>
       <c r="Q5" s="19">
-        <v>1.75</v>
+        <v>1.3</v>
       </c>
       <c r="R5" s="19">
-        <v>1.9</v>
+        <v>1.86</v>
       </c>
       <c r="S5" s="60">
         <v>1E-3</v>
@@ -10628,7 +10628,7 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
forage ub adjusted to 65%, DM AF conversion fixed
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="14490" windowHeight="11160" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="14490" windowHeight="11160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -511,9 +511,6 @@
     <t>Max %DM</t>
   </si>
   <si>
-    <t>Cost [US$/kg AF]</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -986,6 +983,9 @@
   </si>
   <si>
     <t>GSS-MAX_BIS_F_N_2</t>
+  </si>
+  <si>
+    <t>Cost [EUR/kg DM]</t>
   </si>
 </sst>
 </file>
@@ -7361,7 +7361,7 @@
     <tableColumn id="2" name="ID" dataDxfId="71" dataCellStyle="Normal 3"/>
     <tableColumn id="3" name="Min %DM" dataDxfId="70"/>
     <tableColumn id="4" name="Max %DM" dataDxfId="69"/>
-    <tableColumn id="5" name="Cost [US$/kg AF]" dataDxfId="68"/>
+    <tableColumn id="5" name="Cost [EUR/kg DM]" dataDxfId="68"/>
     <tableColumn id="6" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7771,8 +7771,8 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7800,10 +7800,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -8177,7 +8177,7 @@
         <v>100</v>
       </c>
       <c r="E19" s="42">
-        <v>5.2600000000000001E-2</v>
+        <v>0.1</v>
       </c>
       <c r="F19" s="16" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[#Data],2,0)</f>
@@ -8198,7 +8198,7 @@
         <v>100</v>
       </c>
       <c r="E20" s="42">
-        <v>7.6749999999999999E-2</v>
+        <v>0.107</v>
       </c>
       <c r="F20" s="16" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[#Data],2,0)</f>
@@ -8222,8 +8222,8 @@
   </sheetPr>
   <dimension ref="A1:X69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8243,6 +8243,7 @@
     <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.42578125" customWidth="1"/>
     <col min="20" max="20" width="4.85546875" style="2"/>
   </cols>
   <sheetData>
@@ -8254,70 +8255,70 @@
         <v>0</v>
       </c>
       <c r="C1" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="E1" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="F1" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="64" t="s">
-        <v>86</v>
-      </c>
-      <c r="G1" s="65" t="s">
-        <v>87</v>
-      </c>
-      <c r="H1" s="64" t="s">
+      <c r="I1" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="64" t="s">
+      <c r="J1" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="64" t="s">
+      <c r="K1" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="64" t="s">
+      <c r="L1" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="64" t="s">
+      <c r="M1" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="N1" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="64" t="s">
+      <c r="O1" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="64" t="s">
+      <c r="P1" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="64" t="s">
+      <c r="Q1" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="64" t="s">
+      <c r="R1" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="64" t="s">
+      <c r="S1" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="64" t="s">
+      <c r="T1" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="U1" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="64" t="s">
-        <v>89</v>
-      </c>
-      <c r="U1" s="64" t="s">
-        <v>21</v>
-      </c>
       <c r="V1" s="64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="W1" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="X1" s="66" t="s">
         <v>91</v>
-      </c>
-      <c r="X1" s="66" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -8331,7 +8332,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E2" s="19">
         <v>336</v>
@@ -8364,10 +8365,10 @@
         <v>2.41</v>
       </c>
       <c r="O2" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q2" s="19">
         <v>1.33</v>
@@ -8379,10 +8380,10 @@
         <v>0.01</v>
       </c>
       <c r="T2" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V2" s="19">
         <v>0</v>
@@ -8405,7 +8406,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E3" s="19">
         <v>336</v>
@@ -8438,10 +8439,10 @@
         <v>2.41</v>
       </c>
       <c r="O3" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P3" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q3" s="19">
         <v>1.33</v>
@@ -8450,13 +8451,13 @@
         <v>2.02</v>
       </c>
       <c r="S3" s="19">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="T3" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U3" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V3" s="22">
         <v>0</v>
@@ -8479,7 +8480,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E4" s="19">
         <v>336</v>
@@ -8512,10 +8513,10 @@
         <v>2.41</v>
       </c>
       <c r="O4" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P4" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q4" s="19">
         <v>1.33</v>
@@ -8524,13 +8525,13 @@
         <v>2.02</v>
       </c>
       <c r="S4" s="19">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="T4" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U4" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V4" s="22">
         <v>0</v>
@@ -8553,7 +8554,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E5" s="59">
         <v>336</v>
@@ -8586,10 +8587,10 @@
         <v>2.41</v>
       </c>
       <c r="O5" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P5" s="60" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q5" s="19">
         <v>1.33</v>
@@ -8601,10 +8602,10 @@
         <v>0.01</v>
       </c>
       <c r="T5" s="60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U5" s="60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V5" s="60">
         <v>0</v>
@@ -8789,22 +8790,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="F1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -8812,10 +8813,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -8879,61 +8880,61 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="J1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="M1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="O1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="12" t="s">
-        <v>42</v>
-      </c>
       <c r="P1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="12" t="s">
-        <v>46</v>
-      </c>
       <c r="S1" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -8941,7 +8942,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="31">
         <v>0</v>
@@ -9003,7 +9004,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="31">
         <v>0</v>
@@ -9065,7 +9066,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="31">
         <v>0</v>
@@ -9127,7 +9128,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="31">
         <v>0</v>
@@ -9189,7 +9190,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="31">
         <v>0</v>
@@ -9251,7 +9252,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" s="31">
         <v>0</v>
@@ -9313,7 +9314,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="31">
         <v>0</v>
@@ -9375,7 +9376,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="31">
         <v>0</v>
@@ -9437,7 +9438,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C10" s="31">
         <v>0</v>
@@ -9499,7 +9500,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" s="31">
         <v>0</v>
@@ -9561,7 +9562,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C12" s="31">
         <v>0</v>
@@ -9623,7 +9624,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C13" s="31">
         <v>0</v>
@@ -9685,7 +9686,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C14" s="31">
         <v>0</v>
@@ -9747,7 +9748,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15" s="31">
         <v>0</v>
@@ -9809,7 +9810,7 @@
         <v>20</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="31">
         <v>0</v>
@@ -9871,7 +9872,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C17" s="31">
         <v>0</v>
@@ -9933,7 +9934,7 @@
         <v>25</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C18" s="31">
         <v>100</v>
@@ -9995,7 +9996,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C19" s="31">
         <v>0</v>
@@ -10057,7 +10058,7 @@
         <v>29</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" s="31">
         <v>0</v>
@@ -10119,7 +10120,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C21" s="31">
         <v>100</v>
@@ -10181,7 +10182,7 @@
         <v>31</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C22" s="31">
         <v>100</v>
@@ -10319,24 +10320,24 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
@@ -10347,10 +10348,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C3" s="2">
         <v>4</v>
@@ -10361,10 +10362,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" s="2">
         <v>5</v>
@@ -10375,10 +10376,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" s="2">
         <v>6</v>
@@ -10389,10 +10390,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C6" s="2">
         <v>7</v>
@@ -10403,10 +10404,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C7" s="2">
         <v>8</v>
@@ -10417,10 +10418,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C8" s="2">
         <v>9</v>
@@ -10431,10 +10432,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" s="2">
         <v>10</v>
@@ -10445,10 +10446,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C10" s="2">
         <v>11</v>
@@ -10459,10 +10460,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C11" s="2">
         <v>12</v>
@@ -10473,10 +10474,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C12" s="2">
         <v>16</v>
@@ -10487,10 +10488,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C13" s="2">
         <v>17</v>
@@ -10501,10 +10502,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C14" s="2">
         <v>18</v>
@@ -10515,10 +10516,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" s="2">
         <v>19</v>
@@ -10529,10 +10530,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C16" s="2">
         <v>20</v>
@@ -10543,10 +10544,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C17" s="2">
         <v>21</v>
@@ -10557,10 +10558,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C18" s="2">
         <v>25</v>
@@ -10571,10 +10572,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C19" s="2">
         <v>28</v>
@@ -10585,10 +10586,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C20" s="2">
         <v>29</v>
@@ -10599,10 +10600,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C21" s="2">
         <v>30</v>
@@ -10610,10 +10611,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="52" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C22" s="2">
         <v>31</v>
@@ -10656,31 +10657,31 @@
         <v>1</v>
       </c>
       <c r="B1" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="D1" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="E1" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="F1" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="G1" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="H1" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="I1" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="I1" s="58" t="s">
+      <c r="J1" s="58" t="s">
         <v>101</v>
-      </c>
-      <c r="J1" s="58" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -10706,10 +10707,10 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
@@ -10744,10 +10745,10 @@
         <v>0.14285714285714285</v>
       </c>
       <c r="H3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -10782,10 +10783,10 @@
         <v>0.14285714285714285</v>
       </c>
       <c r="H4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J4" t="b">
         <v>0</v>
@@ -10814,10 +10815,10 @@
         <v>0.2</v>
       </c>
       <c r="H5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J5" t="b">
         <v>1</v>
@@ -10846,10 +10847,10 @@
         <v>0.15</v>
       </c>
       <c r="H6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J6" s="2" t="b">
         <v>1</v>
@@ -10892,25 +10893,25 @@
         <v>1</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="E1" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="F1" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="G1" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="H1" s="45" t="s">
         <v>108</v>
-      </c>
-      <c r="H1" s="45" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -10918,7 +10919,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="55">
         <v>5.3300000000000001E-5</v>
@@ -10944,7 +10945,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="56">
         <v>6.5774577999999997E-4</v>
@@ -10970,7 +10971,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="56">
         <v>9.8875607000000008E-4</v>
@@ -10996,7 +10997,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="56">
         <v>4.6734098000000002E-3</v>
@@ -11022,7 +11023,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="56">
         <v>5.2979589999999997E-3</v>
@@ -11048,7 +11049,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" s="56">
         <v>3.0914954E-4</v>
@@ -11074,7 +11075,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="56">
         <v>2.4268531000000001E-3</v>
@@ -11100,7 +11101,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="55">
         <v>1.1524281000000001E-2</v>
@@ -11126,7 +11127,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C10" s="55">
         <v>3.8977495E-3</v>
@@ -11152,7 +11153,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" s="55">
         <v>1.8296865E-3</v>
@@ -11178,7 +11179,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C12" s="55">
         <v>9.5703047000000006E-3</v>
@@ -11204,7 +11205,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C13" s="55">
         <v>1.2856242E-3</v>
@@ -11230,7 +11231,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C14" s="55">
         <v>2.0170432000000001E-3</v>
@@ -11256,7 +11257,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15" s="55">
         <v>6.8793711999999996E-4</v>
@@ -11282,7 +11283,7 @@
         <v>20</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="55">
         <v>1.7751223E-3</v>
@@ -11308,7 +11309,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C17" s="55">
         <v>6.0269407000000002E-4</v>
@@ -11334,7 +11335,7 @@
         <v>25</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C18" s="56">
         <v>1.4474578E-5</v>
@@ -11360,7 +11361,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C19" s="56">
         <v>2.1675339E-3</v>
@@ -11386,7 +11387,7 @@
         <v>29</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" s="55">
         <v>2.1675339E-3</v>
@@ -11412,7 +11413,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="54" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C21" s="57">
         <v>1.4238930000000001E-3</v>
@@ -11438,7 +11439,7 @@
         <v>31</v>
       </c>
       <c r="B22" s="44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C22" s="56">
         <v>1.398646E-5</v>
@@ -11498,287 +11499,287 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
methane factor adjusted 34
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="14490" windowHeight="11160" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="14490" windowHeight="11160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -7771,7 +7771,7 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -8222,8 +8222,8 @@
   </sheetPr>
   <dimension ref="A1:X69"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8323,7 +8323,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B2" s="19">
         <v>1</v>

</xml_diff>

<commit_message>
Docker tidying up and readme update
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="14490" windowHeight="11160" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="14490" windowHeight="11160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -580,7 +580,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="174">
   <si>
     <t>Feed Scenario</t>
   </si>
@@ -1112,13 +1112,20 @@
     <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1314,8 +1321,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1355,6 +1369,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1430,11 +1474,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1442,128 +1486,133 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1572,7 +1621,15 @@
     <cellStyle name="Normal 3" xfId="2"/>
     <cellStyle name="Normal 4" xfId="3"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="68">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2254,34 +2311,34 @@
   </dxfs>
   <tableStyles count="6" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Feeds-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="66"/>
-      <tableStyleElement type="firstRowStripe" dxfId="65"/>
-      <tableStyleElement type="secondRowStripe" dxfId="64"/>
+      <tableStyleElement type="headerRow" dxfId="67"/>
+      <tableStyleElement type="firstRowStripe" dxfId="66"/>
+      <tableStyleElement type="secondRowStripe" dxfId="65"/>
     </tableStyle>
     <tableStyle name="Scenario-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="63"/>
-      <tableStyleElement type="firstRowStripe" dxfId="62"/>
-      <tableStyleElement type="secondRowStripe" dxfId="61"/>
+      <tableStyleElement type="headerRow" dxfId="64"/>
+      <tableStyleElement type="firstRowStripe" dxfId="63"/>
+      <tableStyleElement type="secondRowStripe" dxfId="62"/>
     </tableStyle>
     <tableStyle name="Batch-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="60"/>
-      <tableStyleElement type="firstRowStripe" dxfId="59"/>
-      <tableStyleElement type="secondRowStripe" dxfId="58"/>
+      <tableStyleElement type="headerRow" dxfId="61"/>
+      <tableStyleElement type="firstRowStripe" dxfId="60"/>
+      <tableStyleElement type="secondRowStripe" dxfId="59"/>
     </tableStyle>
     <tableStyle name="Feed Library-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="57"/>
-      <tableStyleElement type="firstRowStripe" dxfId="56"/>
-      <tableStyleElement type="secondRowStripe" dxfId="55"/>
+      <tableStyleElement type="headerRow" dxfId="58"/>
+      <tableStyleElement type="firstRowStripe" dxfId="57"/>
+      <tableStyleElement type="secondRowStripe" dxfId="56"/>
     </tableStyle>
     <tableStyle name="LCA-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="54"/>
-      <tableStyleElement type="firstRowStripe" dxfId="53"/>
-      <tableStyleElement type="secondRowStripe" dxfId="52"/>
+      <tableStyleElement type="headerRow" dxfId="55"/>
+      <tableStyleElement type="firstRowStripe" dxfId="54"/>
+      <tableStyleElement type="secondRowStripe" dxfId="53"/>
     </tableStyle>
     <tableStyle name="LCA Library-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="51"/>
-      <tableStyleElement type="firstRowStripe" dxfId="50"/>
-      <tableStyleElement type="secondRowStripe" dxfId="49"/>
+      <tableStyleElement type="headerRow" dxfId="52"/>
+      <tableStyleElement type="firstRowStripe" dxfId="51"/>
+      <tableStyleElement type="secondRowStripe" dxfId="50"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -6700,10 +6757,10 @@
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="Feed Scenario"/>
-    <tableColumn id="2" name="ID" dataDxfId="48" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Min %DM" dataDxfId="47"/>
-    <tableColumn id="4" name="Max %DM" dataDxfId="46"/>
-    <tableColumn id="5" name="Cost [EUR/kg DM]" dataDxfId="45"/>
+    <tableColumn id="2" name="ID" dataDxfId="49" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Min %DM" dataDxfId="48"/>
+    <tableColumn id="4" name="Max %DM" dataDxfId="47"/>
+    <tableColumn id="5" name="Cost [EUR/kg DM]" dataDxfId="46"/>
     <tableColumn id="6" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6711,7 +6768,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="scenario" displayName="scenario" ref="A1:Y4" totalsRowShown="0" headerRowDxfId="44" tableBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="scenario" displayName="scenario" ref="A1:Y4" totalsRowShown="0" headerRowDxfId="45" tableBorderDxfId="44">
   <autoFilter ref="A1:Y4"/>
   <tableColumns count="25">
     <tableColumn id="1" name="ID"/>
@@ -6760,32 +6817,32 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:T23" totalsRowShown="0" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:T23" totalsRowShown="0" dataDxfId="39">
   <autoFilter ref="A1:T23"/>
   <sortState ref="A2:T22">
     <sortCondition ref="A1:A22"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="ID" dataDxfId="37"/>
-    <tableColumn id="2" name="Feed" dataDxfId="36"/>
-    <tableColumn id="5" name="Forage, %DM" dataDxfId="35"/>
-    <tableColumn id="6" name="DM, %AF" dataDxfId="34"/>
-    <tableColumn id="7" name="CP, %DM" dataDxfId="33"/>
-    <tableColumn id="8" name="SP, %CP" dataDxfId="32"/>
-    <tableColumn id="9" name="ADICP, %CP" dataDxfId="31"/>
-    <tableColumn id="10" name="Sugars, %DM" dataDxfId="30"/>
-    <tableColumn id="11" name="OA, %DM" dataDxfId="29"/>
-    <tableColumn id="12" name="Fat, %DM" dataDxfId="28"/>
-    <tableColumn id="13" name="Ash, %DM" dataDxfId="27"/>
-    <tableColumn id="14" name="Starch, %DM" dataDxfId="26"/>
-    <tableColumn id="15" name="NDF, %DM" dataDxfId="25"/>
-    <tableColumn id="16" name="Lignin, %DM" dataDxfId="24"/>
-    <tableColumn id="17" name="TDN, %DM" dataDxfId="23"/>
-    <tableColumn id="19" name="NEma, Mcal/kg" dataDxfId="22"/>
-    <tableColumn id="20" name="NEga, Mcal/kg" dataDxfId="21"/>
-    <tableColumn id="21" name="RUP, %CP" dataDxfId="20"/>
-    <tableColumn id="29" name="pef, %NDF" dataDxfId="19"/>
-    <tableColumn id="3" name="NPN, %DM" dataDxfId="18"/>
+    <tableColumn id="1" name="ID" dataDxfId="38"/>
+    <tableColumn id="2" name="Feed" dataDxfId="37"/>
+    <tableColumn id="5" name="Forage, %DM" dataDxfId="36"/>
+    <tableColumn id="6" name="DM, %AF" dataDxfId="35"/>
+    <tableColumn id="7" name="CP, %DM" dataDxfId="34"/>
+    <tableColumn id="8" name="SP, %CP" dataDxfId="33"/>
+    <tableColumn id="9" name="ADICP, %CP" dataDxfId="32"/>
+    <tableColumn id="10" name="Sugars, %DM" dataDxfId="31"/>
+    <tableColumn id="11" name="OA, %DM" dataDxfId="30"/>
+    <tableColumn id="12" name="Fat, %DM" dataDxfId="29"/>
+    <tableColumn id="13" name="Ash, %DM" dataDxfId="28"/>
+    <tableColumn id="14" name="Starch, %DM" dataDxfId="27"/>
+    <tableColumn id="15" name="NDF, %DM" dataDxfId="26"/>
+    <tableColumn id="16" name="Lignin, %DM" dataDxfId="25"/>
+    <tableColumn id="17" name="TDN, %DM" dataDxfId="24"/>
+    <tableColumn id="19" name="NEma, Mcal/kg" dataDxfId="23"/>
+    <tableColumn id="20" name="NEga, Mcal/kg" dataDxfId="22"/>
+    <tableColumn id="21" name="RUP, %CP" dataDxfId="21"/>
+    <tableColumn id="29" name="pef, %NDF" dataDxfId="20"/>
+    <tableColumn id="3" name="NPN, %DM" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6798,7 +6855,7 @@
     <sortCondition ref="C1:C22"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name INRA" dataDxfId="15"/>
+    <tableColumn id="1" name="Name INRA" dataDxfId="16"/>
     <tableColumn id="2" name="Name RNS"/>
     <tableColumn id="3" name="ID"/>
     <tableColumn id="4" name="Column1"/>
@@ -6808,7 +6865,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="lca" displayName="lca" ref="A1:N3" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="lca" displayName="lca" ref="A1:N3" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A1:N3"/>
   <tableColumns count="14">
     <tableColumn id="1" name="ID"/>
@@ -6821,7 +6878,7 @@
     <tableColumn id="14" name="Methane_Equation"/>
     <tableColumn id="7" name="N2O_Equation"/>
     <tableColumn id="2" name="Normalize"/>
-    <tableColumn id="4" name="EI_weight" dataDxfId="13" dataCellStyle="Normal 2"/>
+    <tableColumn id="4" name="EI_weight" dataDxfId="14" dataCellStyle="Normal 2"/>
     <tableColumn id="6" name="Profit_weight" dataCellStyle="Normal 2"/>
     <tableColumn id="8" name="EI_REF to compute carbon profit" dataCellStyle="Normal 2"/>
     <tableColumn id="13" name="Carbon Cost (per kg CO2eq)" dataCellStyle="Normal 2"/>
@@ -6831,28 +6888,28 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela26" displayName="Tabela26" ref="A1:I23" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela26" displayName="Tabela26" ref="A1:I23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:I23"/>
   <sortState ref="A2:H22">
     <sortCondition ref="A1:A22"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" name="ID" dataDxfId="8" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Name" dataDxfId="7" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" name="LCA_Phosphorous consumption (kg P)" dataDxfId="6"/>
-    <tableColumn id="3" name="LCA_CED 1.8 non renewable fossil+nuclear (MJ)" dataDxfId="5"/>
-    <tableColumn id="4" name="LCA_Climate change ILCD (kg CO2 eq)" dataDxfId="4"/>
-    <tableColumn id="7" name="LCA_Acidification ILCD (molc H+ eq)" dataDxfId="3"/>
-    <tableColumn id="8" name="LCA_Eutrophication CML baseline (kg PO4- eq)" dataDxfId="2"/>
-    <tableColumn id="9" name="LCA_Land competition CML non baseline (m2a)" dataDxfId="1"/>
-    <tableColumn id="6" name="Carbon Cost Bool" dataDxfId="0"/>
+    <tableColumn id="1" name="ID" dataDxfId="9" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Name" dataDxfId="8" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" name="LCA_Phosphorous consumption (kg P)" dataDxfId="7"/>
+    <tableColumn id="3" name="LCA_CED 1.8 non renewable fossil+nuclear (MJ)" dataDxfId="6"/>
+    <tableColumn id="4" name="LCA_Climate change ILCD (kg CO2 eq)" dataDxfId="5"/>
+    <tableColumn id="7" name="LCA_Acidification ILCD (molc H+ eq)" dataDxfId="4"/>
+    <tableColumn id="8" name="LCA_Eutrophication CML baseline (kg PO4- eq)" dataDxfId="3"/>
+    <tableColumn id="9" name="LCA_Land competition CML non baseline (m2a)" dataDxfId="2"/>
+    <tableColumn id="6" name="Carbon Cost Bool" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:E3" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:E3" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:E3"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Additive Scenario"/>
@@ -7573,7 +7630,7 @@
       <c r="A21">
         <v>1</v>
       </c>
-      <c r="B21" s="62">
+      <c r="B21" s="59">
         <v>99</v>
       </c>
       <c r="C21" s="17">
@@ -7582,7 +7639,7 @@
       <c r="D21" s="22">
         <v>100</v>
       </c>
-      <c r="E21" s="63">
+      <c r="E21" s="60">
         <v>3</v>
       </c>
       <c r="F21" t="s">
@@ -7606,8 +7663,8 @@
   </sheetPr>
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7631,6 +7688,7 @@
     <col min="20" max="20" width="4.85546875" style="2"/>
     <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7697,16 +7755,16 @@
       <c r="U1" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="54" t="s">
+      <c r="V1" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="W1" s="54" t="s">
+      <c r="W1" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="X1" s="56" t="s">
+      <c r="X1" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="Y1" s="67" t="s">
+      <c r="Y1" s="68" t="s">
         <v>168</v>
       </c>
     </row>
@@ -7852,7 +7910,7 @@
         <v>87</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="W3">
         <v>0.1</v>
@@ -7942,7 +8000,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -9427,7 +9485,7 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="61">
+      <c r="A23" s="58">
         <v>99</v>
       </c>
       <c r="B23" s="38" t="s">
@@ -9528,18 +9586,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B19 B2:I18">
-    <cfRule type="expression" dxfId="42" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="3" stopIfTrue="1">
       <formula>ROW(B2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="4" stopIfTrue="1">
       <formula>COLUMN(B2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:I19">
-    <cfRule type="expression" dxfId="40" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="6" stopIfTrue="1">
       <formula>COLUMN(C19)=$F$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="9" stopIfTrue="1">
       <formula>ROW(C19)=$E$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9872,10 +9930,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A19">
-    <cfRule type="expression" dxfId="17" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="12" stopIfTrue="1">
       <formula>ROW(A2)=$D$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="13" stopIfTrue="1">
       <formula>COLUMN(A2)=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9893,8 +9951,8 @@
   </sheetPr>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9933,16 +9991,16 @@
       <c r="J1" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="K1" s="71" t="s">
         <v>160</v>
       </c>
-      <c r="L1" s="58" t="s">
+      <c r="L1" s="72" t="s">
         <v>161</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="N1" s="64" t="s">
+      <c r="N1" s="69" t="s">
         <v>163</v>
       </c>
     </row>
@@ -9977,13 +10035,13 @@
       <c r="J2" t="b">
         <v>0</v>
       </c>
-      <c r="K2" s="65">
+      <c r="K2" s="61">
         <v>1</v>
       </c>
       <c r="L2" s="18">
-        <v>1</v>
-      </c>
-      <c r="M2" s="66">
+        <v>0</v>
+      </c>
+      <c r="M2" s="62">
         <v>1.8153428621454899</v>
       </c>
       <c r="N2" s="18">
@@ -10021,16 +10079,16 @@
       <c r="J3" t="b">
         <v>0</v>
       </c>
-      <c r="K3" s="18">
-        <v>0</v>
-      </c>
-      <c r="L3" s="18">
-        <v>1</v>
-      </c>
-      <c r="M3" s="65" t="s">
+      <c r="K3" s="65" t="s">
         <v>167</v>
       </c>
-      <c r="N3" s="65" t="s">
+      <c r="L3" s="65" t="s">
+        <v>167</v>
+      </c>
+      <c r="M3" s="61" t="s">
+        <v>167</v>
+      </c>
+      <c r="N3" s="61" t="s">
         <v>167</v>
       </c>
     </row>
@@ -10104,7 +10162,7 @@
       <c r="H1" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="64" t="s">
         <v>173</v>
       </c>
     </row>
@@ -10133,7 +10191,7 @@
       <c r="H2" s="50">
         <v>8.2600000000000007E-2</v>
       </c>
-      <c r="I2" s="59" t="b">
+      <c r="I2" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10162,7 +10220,7 @@
       <c r="H3" s="51">
         <v>0.55197054999999995</v>
       </c>
-      <c r="I3" s="59" t="b">
+      <c r="I3" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10191,7 +10249,7 @@
       <c r="H4" s="51">
         <v>0.43937693999999999</v>
       </c>
-      <c r="I4" s="59" t="b">
+      <c r="I4" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10220,7 +10278,7 @@
       <c r="H5" s="51">
         <v>2.0767392</v>
       </c>
-      <c r="I5" s="59" t="b">
+      <c r="I5" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10249,7 +10307,7 @@
       <c r="H6" s="51">
         <v>2.4169052999999998</v>
       </c>
-      <c r="I6" s="59" t="b">
+      <c r="I6" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10278,7 +10336,7 @@
       <c r="H7" s="51">
         <v>0.25908868000000002</v>
       </c>
-      <c r="I7" s="59" t="b">
+      <c r="I7" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10307,7 +10365,7 @@
       <c r="H8" s="51">
         <v>1.2147266999999999</v>
       </c>
-      <c r="I8" s="59" t="b">
+      <c r="I8" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10336,7 +10394,7 @@
       <c r="H9" s="50">
         <v>5.7683147000000004</v>
       </c>
-      <c r="I9" s="59" t="b">
+      <c r="I9" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10365,7 +10423,7 @@
       <c r="H10" s="50">
         <v>3.8084742</v>
       </c>
-      <c r="I10" s="59" t="b">
+      <c r="I10" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10394,7 +10452,7 @@
       <c r="H11" s="50">
         <v>1.6645894999999999</v>
       </c>
-      <c r="I11" s="59" t="b">
+      <c r="I11" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10423,7 +10481,7 @@
       <c r="H12" s="50">
         <v>8.7067530000000009</v>
       </c>
-      <c r="I12" s="59" t="b">
+      <c r="I12" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10452,7 +10510,7 @@
       <c r="H13" s="50">
         <v>0.62333822000000005</v>
       </c>
-      <c r="I13" s="59" t="b">
+      <c r="I13" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10481,7 +10539,7 @@
       <c r="H14" s="50">
         <v>0.97791181999999999</v>
       </c>
-      <c r="I14" s="59" t="b">
+      <c r="I14" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10510,7 +10568,7 @@
       <c r="H15" s="50">
         <v>0.33293109999999998</v>
       </c>
-      <c r="I15" s="59" t="b">
+      <c r="I15" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10539,7 +10597,7 @@
       <c r="H16" s="50">
         <v>0.86067262</v>
       </c>
-      <c r="I16" s="59" t="b">
+      <c r="I16" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10568,7 +10626,7 @@
       <c r="H17" s="50">
         <v>0.29167724</v>
       </c>
-      <c r="I17" s="59" t="b">
+      <c r="I17" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10597,7 +10655,7 @@
       <c r="H18" s="51">
         <v>1.1395907999999999</v>
       </c>
-      <c r="I18" s="59" t="b">
+      <c r="I18" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10626,7 +10684,7 @@
       <c r="H19" s="51">
         <v>1.9759963</v>
       </c>
-      <c r="I19" s="59" t="b">
+      <c r="I19" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10655,7 +10713,7 @@
       <c r="H20" s="50">
         <v>1.9759963</v>
       </c>
-      <c r="I20" s="59" t="b">
+      <c r="I20" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10684,7 +10742,7 @@
       <c r="H21" s="52">
         <v>0.89059001000000004</v>
       </c>
-      <c r="I21" s="59" t="b">
+      <c r="I21" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10713,7 +10771,7 @@
       <c r="H22" s="51">
         <v>1.1594272000000001</v>
       </c>
-      <c r="I22" s="59" t="b">
+      <c r="I22" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10721,37 +10779,37 @@
       <c r="A23" s="48">
         <v>99</v>
       </c>
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="C23" s="59">
-        <v>0</v>
-      </c>
-      <c r="D23" s="59">
-        <v>0</v>
-      </c>
-      <c r="E23" s="59">
+      <c r="C23" s="56">
+        <v>0</v>
+      </c>
+      <c r="D23" s="56">
+        <v>0</v>
+      </c>
+      <c r="E23" s="56">
         <v>0.6</v>
       </c>
-      <c r="F23" s="59">
-        <v>0</v>
-      </c>
-      <c r="G23" s="59">
-        <v>0</v>
-      </c>
-      <c r="H23" s="59">
-        <v>0</v>
-      </c>
-      <c r="I23" s="59" t="b">
+      <c r="F23" s="56">
+        <v>0</v>
+      </c>
+      <c r="G23" s="56">
+        <v>0</v>
+      </c>
+      <c r="H23" s="56">
+        <v>0</v>
+      </c>
+      <c r="I23" s="56" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A19:A21 A2:A16">
-    <cfRule type="expression" dxfId="12" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="3" stopIfTrue="1">
       <formula>ROW(A2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="4" stopIfTrue="1">
       <formula>COLUMN(A2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10766,12 +10824,12 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10782,19 +10840,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="70" t="s">
         <v>170</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="70" t="s">
         <v>169</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="70" t="s">
         <v>171</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="70" t="s">
         <v>172</v>
       </c>
     </row>
@@ -10818,7 +10876,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>99</v>
@@ -10830,7 +10888,7 @@
       <c r="D3" s="2">
         <v>0.01</v>
       </c>
-      <c r="E3" s="68">
+      <c r="E3" s="63">
         <v>0.17</v>
       </c>
     </row>

</xml_diff>